<commit_message>
ccbottlersus, change survey of Value2 and fix same_pack function
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/Data/SurveyTemplateV2.xlsx
+++ b/Projects/CCBOTTLERSUS/Data/SurveyTemplateV2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,1773 +26,1773 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="589">
   <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>store_type</t>
-  </si>
-  <si>
-    <t>KPI_name</t>
-  </si>
-  <si>
-    <t>display_text</t>
-  </si>
-  <si>
-    <t>condition</t>
-  </si>
-  <si>
-    <t>group_target</t>
-  </si>
-  <si>
-    <t>incremental</t>
-  </si>
-  <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>UNITED</t>
-  </si>
-  <si>
-    <t>CR&amp;LT</t>
-  </si>
-  <si>
-    <t>CR&amp;LT1</t>
-  </si>
-  <si>
-    <t>PICOS POI # 1:Do we have a Coke branded cooler in the Impulse Zone?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT1a</t>
-  </si>
-  <si>
-    <t>1a.Is 2018 Innovation available in the Impulse Zone area, either in an FLM or ice barrel?”</t>
-  </si>
-  <si>
-    <t>CR&amp;LT1b</t>
-  </si>
-  <si>
-    <t>1b.Are all the 20oz SSD core brands plus Dasani 20oz represented in the Impulse Zone cooler?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT2</t>
-  </si>
-  <si>
-    <t>PICOS POI # 2:Is there a Sparkling can display?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT2a</t>
-  </si>
-  <si>
-    <t>2a.Are all core brands on display?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT2b</t>
-  </si>
-  <si>
-    <t>2b.Is Dasani 12pk 12oz on display?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT3</t>
-  </si>
-  <si>
-    <t>PICOS POI # 3:Is there a Powerade Display in this outlet (any pkg)?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT4</t>
-  </si>
-  <si>
-    <t>PICOS POI # 4:Is there an incrementalBranded (Monster, NOS or Full Throttle graphics) Energy Coolerin this outlet?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT5</t>
-  </si>
-  <si>
-    <t>PICOS POI # 5:Is there a Sparkling PET display?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT5a</t>
-  </si>
-  <si>
-    <t>5a.Are all core brands on display?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT6</t>
-  </si>
-  <si>
-    <t>PICOS POI #6:Is there a Still Displayexcluding Dasani Casepack Waterin this outlet?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT7</t>
-  </si>
-  <si>
-    <t>PICOS POI # 7:Is there an incremental SmartWater Display or Rack in this outlet?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT8</t>
-  </si>
-  <si>
-    <t>PICOS POI # 8:Is there a Branded Coffee Cooler in this outlet ?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT9</t>
-  </si>
-  <si>
-    <t>PICOS POI # 9:Do we have a Coke branded barrel, ice chest or incremental Coke identified cooler (cold availability) in the outlet?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT10</t>
-  </si>
-  <si>
-    <t>PICOS POI # 10:Is there a Coke Identified Fountain in this outlet with pricing POS available (never on logo panel)?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT11</t>
-  </si>
-  <si>
-    <t>PICOS POI # 11:Is Gold Peak brewed tea, brewed coffee or tea tower available in this outlet?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT12</t>
-  </si>
-  <si>
-    <t>12:Are all authorized SPK and Still CCBCU products available and ready for sale?  Take a picture and add a comment for each OOS. Capture all OOS instances in the OOS feature while conducting the survey.</t>
-  </si>
-  <si>
-    <t>CR&amp;LT13</t>
-  </si>
-  <si>
-    <t>13:Is there a Premium SSD package offered cold in the outlet (8oz, 12oz glass, 8.5 oz aluminum or Import glass)?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT14</t>
-  </si>
-  <si>
-    <t>14:Are there 5 flavors of Gold Peak 18.5oz"cold"available in this outlet?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT15</t>
-  </si>
-  <si>
-    <t>15:Are there 5 flavors of Fanta 20oz"cold"available in this outlet?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT16</t>
-  </si>
-  <si>
-    <t>16:Are there 2+ packages of SmartWater available in this outlet?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT17</t>
-  </si>
-  <si>
-    <t>17:Are there 2+ packages of Dasani available in this outlet?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT18</t>
-  </si>
-  <si>
-    <t>18:Is Sparkling Can display in best position?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT19</t>
-  </si>
-  <si>
-    <t>19:Is Sparkling PET display in best position?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT20</t>
-  </si>
-  <si>
-    <t>20:Is Still Display(excluding Dasani Casepack Water)in best position?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT21</t>
-  </si>
-  <si>
-    <t>21: PICOS POI -Is the KO SSD messaging "Taste the Feeling" for sparkling IC core brand package visible from the outside?SSD IC Pkg./Price will vary.</t>
-  </si>
-  <si>
-    <t>CR&amp;LT22</t>
-  </si>
-  <si>
-    <t>22:Are there a minimum 5 SSD POIfrom curb to cold vault?("Taste the Feeling" for sparkling IC core brand package)</t>
-  </si>
-  <si>
-    <t>CR&amp;LT23</t>
-  </si>
-  <si>
-    <t>23: PICOS POI -Is there aFood Solutionwith SSD in this outlet?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT24</t>
-  </si>
-  <si>
-    <t>24:Are Coca-Cola identified fountain cups available in this outlet?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT25</t>
-  </si>
-  <si>
-    <t>25: PICOS POI -Are there a minimum 3 Monster POIs from curb to cold vault?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT26</t>
-  </si>
-  <si>
-    <t>26:Are all displays properly priced?</t>
-  </si>
-  <si>
-    <t>CR&amp;LT27</t>
-  </si>
-  <si>
-    <t>27:Are all SKUs in cold vault/equipment properly priced?</t>
-  </si>
-  <si>
-    <t>Drug</t>
-  </si>
-  <si>
-    <t>Drug1</t>
-  </si>
-  <si>
-    <t>1:Is there a Coke SSD FEM / FLM in this outlet?</t>
-  </si>
-  <si>
-    <t>Drug1a</t>
-  </si>
-  <si>
-    <t>1a:Do we have a Coke cooler in checkout area of the outlet?</t>
-  </si>
-  <si>
-    <t>Drug1b</t>
-  </si>
-  <si>
-    <t>1b:Are all the 20oz SSD core brands plus Dasani 20oz represented in the cooler?</t>
-  </si>
-  <si>
-    <t>Drug1c</t>
-  </si>
-  <si>
-    <t>1c:Is the FLM cooler and cold vault space if available priced correctly?</t>
-  </si>
-  <si>
-    <t>Drug2</t>
-  </si>
-  <si>
-    <t>2:Is there a SmartWater Rack incremental tofirststill display in this outlet?</t>
-  </si>
-  <si>
-    <t>Drug3</t>
-  </si>
-  <si>
-    <t>3:Is there a free standing ambient water rack in or around the pharmacy?</t>
-  </si>
-  <si>
-    <t>Drug4</t>
-  </si>
-  <si>
-    <t>4:Is there a Transaction Package Display present in the store?</t>
-  </si>
-  <si>
-    <t>Drug5</t>
-  </si>
-  <si>
-    <t>5:Is there a Still Display in this outlet?</t>
-  </si>
-  <si>
-    <t>Drug6</t>
-  </si>
-  <si>
-    <t>6:Is there a Sparkling Display in this outlet?</t>
-  </si>
-  <si>
-    <t>Drug6a</t>
-  </si>
-  <si>
-    <t>6a.Are all core brands available?</t>
-  </si>
-  <si>
-    <t>Drug7</t>
-  </si>
-  <si>
-    <t>7:Are the Gold Peak multipack or Gold Peak 64 oz or Honest Tea 59 oz available in the warm section?</t>
-  </si>
-  <si>
-    <t>Drug8</t>
-  </si>
-  <si>
-    <t>8:Is Dasani Sparkling available?</t>
-  </si>
-  <si>
-    <t>Drug9</t>
-  </si>
-  <si>
-    <t>9:Are Dasani 20oz &amp; 1 Liter available?</t>
-  </si>
-  <si>
-    <t>Drug10</t>
-  </si>
-  <si>
-    <t>10:Is Powerade 4 pk. 20 oz or 6pk 12oz available?</t>
-  </si>
-  <si>
-    <t>Drug11</t>
-  </si>
-  <si>
-    <t>11:Are 4 SKUs of Dunkin or McCafe available?</t>
-  </si>
-  <si>
-    <t>Drug12</t>
-  </si>
-  <si>
-    <t>Drug13</t>
-  </si>
-  <si>
-    <t>13:If there is a Coke SSD FEM/FLM in this outlet, is it in first position?</t>
-  </si>
-  <si>
-    <t>Drug14</t>
-  </si>
-  <si>
-    <t>14. If there is a Sparkling display in this outlet, is it in best position?</t>
-  </si>
-  <si>
-    <t>Drug15</t>
-  </si>
-  <si>
-    <t>15.Are all displays properly priced?</t>
-  </si>
-  <si>
-    <t>Supermarket</t>
-  </si>
-  <si>
-    <t>Supermarket1</t>
-  </si>
-  <si>
-    <t>PICOSPOI # 1:Sparkling Display #1: Is there a SSD display in this outlet?  SSD Transaction Package must be included.  Still is optional.</t>
-  </si>
-  <si>
-    <t>Supermarket1a</t>
-  </si>
-  <si>
-    <t>1a.Is there a SSD transaction package co-merchandised?</t>
-  </si>
-  <si>
-    <t>Supermarket1b</t>
-  </si>
-  <si>
-    <t>1b.Are all core brands available?</t>
-  </si>
-  <si>
-    <t>Supermarket2</t>
-  </si>
-  <si>
-    <t>PICOSPOI # 2:Still HydrationDisplay # 1 (Include Water and/or PowerAde).Is there a Hydration Still display that includes water and/orPowerade?</t>
-  </si>
-  <si>
-    <t>Supermarket2a</t>
-  </si>
-  <si>
-    <t>2a. If a Water Display Is Dasani sparkling co-merchandised or if Sports Display is PowerAde multi-pack co-merchandised?</t>
-  </si>
-  <si>
-    <t>Supermarket3</t>
-  </si>
-  <si>
-    <t>PICOSPOI # 3:Sparkling Display #2: Is there a SSD display in this outlet?SSD Transaction Package must be included.</t>
-  </si>
-  <si>
-    <t>Supermarket3a</t>
-  </si>
-  <si>
-    <t>3a.Does display include SSD transaction packages?</t>
-  </si>
-  <si>
-    <t>Supermarket3b</t>
-  </si>
-  <si>
-    <t>3b.Are all core brands available?</t>
-  </si>
-  <si>
-    <t>Supermarket4</t>
-  </si>
-  <si>
-    <t>PICOS POI #4.Do we have KO cold availability in self checkoutand/orexpress checkout ?</t>
-  </si>
-  <si>
-    <t>Supermarket4a</t>
-  </si>
-  <si>
-    <t>4a.Is 20oz KO Sparkling and Dasani available in all 20 oz FLM coolers ?</t>
-  </si>
-  <si>
-    <t>Supermarket5</t>
-  </si>
-  <si>
-    <t>PICOS POI # 5 :Is there an incremental Minican Display in the outlet?  Minimum Display of 6 cases with at least 4 brands on display.</t>
-  </si>
-  <si>
-    <t>Supermarket6</t>
-  </si>
-  <si>
-    <t>PICOSPOI # 6:Still HydrationDisplay # 2 (Include Water and/or PowerAde).Is there a Hydration Still display that includes water and/orPowerade?</t>
-  </si>
-  <si>
-    <t>Supermarket6a</t>
-  </si>
-  <si>
-    <t>6a. If a Water Display Is Dasani Sparkling co-merchandised or if Sports Display is PowerAde multi-pack co-merchandised?</t>
-  </si>
-  <si>
-    <t>Supermarket7</t>
-  </si>
-  <si>
-    <t>PICOS POI # 7:Is there an incremental Sparkling non Cola or Flavor Display in this outlet?Brand Options include:  Fanta / Sprite / Mello Yello / Barqs</t>
-  </si>
-  <si>
-    <t>Supermarket8</t>
-  </si>
-  <si>
-    <t>PICOS POI # 8:Is there a SmartWaterRackor Display incremental to Hydration displays #1 &amp; #2 in this outlet?</t>
-  </si>
-  <si>
-    <t>Supermarket9</t>
-  </si>
-  <si>
-    <t>PICOSPOI # 9:Is there a Meal Combo with SSD and Gold Peak Tea executed in this outlet ?</t>
-  </si>
-  <si>
-    <t>Supermarket10</t>
-  </si>
-  <si>
-    <t>PICOSPOI # 10:Is there a Coca-Cola Sparkling with a SnackBundlein this outlet?</t>
-  </si>
-  <si>
-    <t>Supermarket11</t>
-  </si>
-  <si>
-    <t>PICOSPOI # 11:Is there aGold Peak Tearack/display in the outlet?</t>
-  </si>
-  <si>
-    <t>Supermarket12</t>
-  </si>
-  <si>
-    <t>PICOS POI # 12:Is there an Energy (Monster, Full Throttle or NOS) Display or Cooler executed in this outlet?</t>
-  </si>
-  <si>
-    <t>Supermarket13</t>
-  </si>
-  <si>
-    <t>PICOS POI # 13  Is there a Coffee Display, Rack or Cooler executed in this outlet?</t>
-  </si>
-  <si>
-    <t>Supermarket14</t>
-  </si>
-  <si>
-    <t>PICOSPOI # 14:Is there an incremental Premium SSD package display or rack in the outlet (8oz glass,12 oz 4pk, 12oz 6pk,8.5oz aluminum or Import glass) ?</t>
-  </si>
-  <si>
-    <t>Supermarket15</t>
-  </si>
-  <si>
-    <t>PICOS POI # 15:Is there a Dasani Sparkling water display in this outlet?  Display must include at least 4 flavors.</t>
-  </si>
-  <si>
-    <t>Supermarket16</t>
-  </si>
-  <si>
-    <t>PICOS POI # 16:  Is there a Hydrate and Recover Display in this outlet?  Brands must include both PowerAde and Core Power.</t>
-  </si>
-  <si>
-    <t>Supermarket17</t>
-  </si>
-  <si>
-    <t>17.Are all authorized SPK and Still CCBCU products available and ready for sale?  Take a picture and add a comment for each OOS. Capture all OOS instances in the OOS feature while conducting the survey.</t>
-  </si>
-  <si>
-    <t>Supermarket18</t>
-  </si>
-  <si>
-    <t>18.Are all displays properly priced?</t>
-  </si>
-  <si>
-    <t>Supermarket19</t>
-  </si>
-  <si>
-    <t>19.Are all SKUs in cold door equipment properly priced?</t>
-  </si>
-  <si>
-    <t>Supermarket20</t>
-  </si>
-  <si>
-    <t>20:Are the beverage aisle shelf tag retails matching display retails?</t>
-  </si>
-  <si>
-    <t>Supermarket21</t>
-  </si>
-  <si>
-    <t>21.Is there an SSD display in quad 1?</t>
-  </si>
-  <si>
-    <t>Supermarket22</t>
-  </si>
-  <si>
-    <t>22.Is SSD display in quad 1 in best position?</t>
-  </si>
-  <si>
-    <t>Supermarket23</t>
-  </si>
-  <si>
-    <t>23.Is Still Hydration display #1 in best position?</t>
-  </si>
-  <si>
-    <t>Supermarket24</t>
-  </si>
-  <si>
-    <t>24.Are Front-End FLM /Coolers with our products in the Best position in the checkout area &gt; = primary competition?</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Value1</t>
-  </si>
-  <si>
-    <t>Value1a</t>
-  </si>
-  <si>
-    <t>1a.Are Monster Energy products available in Coke FEM / FLM?</t>
-  </si>
-  <si>
-    <t>Value2</t>
-  </si>
-  <si>
-    <t>2:Is there a Sparkling Display in this outlet?</t>
-  </si>
-  <si>
-    <t>Value2a</t>
-  </si>
-  <si>
-    <t>2a.Are all core brands available?</t>
-  </si>
-  <si>
-    <t>Value3</t>
-  </si>
-  <si>
-    <t>3:Is there a Transactional Pkg Sparkling Display in this outlet?</t>
-  </si>
-  <si>
-    <t>Value4</t>
-  </si>
-  <si>
-    <t>4:Is there a Sparkling Flavor Future Consumption Display in this outlet?</t>
-  </si>
-  <si>
-    <t>Value5</t>
-  </si>
-  <si>
-    <t>Value6</t>
-  </si>
-  <si>
-    <t>6:Are all authorized SPK and Still CCBCU products available and ready for sale?  Take a picture and add a comment for each OOS.  Capture all OOS instances in the OOS feature while conducting the survey.</t>
-  </si>
-  <si>
-    <t>Value7</t>
-  </si>
-  <si>
-    <t>7:Are Monster Multipacks available in the warm set?</t>
-  </si>
-  <si>
-    <t>Value8</t>
-  </si>
-  <si>
-    <t>8:Is Gold Peak 18.5oz available in the Still Section?</t>
-  </si>
-  <si>
-    <t>Value9</t>
-  </si>
-  <si>
-    <t>9:Is SmartWater 1 Liter and/or 700 ml available in the Still Section?</t>
-  </si>
-  <si>
-    <t>Value10</t>
-  </si>
-  <si>
-    <t>10:Are Dasani 20oz &amp; 1 Liter available?</t>
-  </si>
-  <si>
-    <t>Value11</t>
-  </si>
-  <si>
-    <t>11:Is Powerade 4pk. 20oz or 6pk 12oz available?</t>
-  </si>
-  <si>
-    <t>Value12</t>
-  </si>
-  <si>
-    <t>12:Are two SKUs of McCafe available?</t>
-  </si>
-  <si>
-    <t>Value13</t>
-  </si>
-  <si>
-    <t>13.If there is a Sparkling display in this outlet, is display in best position?</t>
-  </si>
-  <si>
-    <t>Value14</t>
-  </si>
-  <si>
-    <t>14.Are all displays properly priced?</t>
-  </si>
-  <si>
-    <t>Value15</t>
-  </si>
-  <si>
-    <t>15.Are all beverage aisle SKUs properly priced?</t>
-  </si>
-  <si>
-    <t>Value16</t>
-  </si>
-  <si>
-    <t>16.All cold equipment properly priced?</t>
-  </si>
-  <si>
-    <t>WMNH</t>
-  </si>
-  <si>
-    <t>WMNH1</t>
-  </si>
-  <si>
-    <t>Question 1: Is there a Core Can End Cap/Display in this outlet ?</t>
-  </si>
-  <si>
-    <t>WMNH1a</t>
-  </si>
-  <si>
-    <t>1a.Are all core brands available?</t>
-  </si>
-  <si>
-    <t>WMNH2</t>
-  </si>
-  <si>
-    <t>Question 2:Is there a SSD Flavor program executed in this outlet ?</t>
-  </si>
-  <si>
-    <t>WMNH3</t>
-  </si>
-  <si>
-    <t>Question 3:Is  there an SSD display in the outlet with one of the following transaction packages; (mini-cans, 6pk 500ml, 8pk 12oz)?</t>
-  </si>
-  <si>
-    <t>WMNH3a</t>
-  </si>
-  <si>
-    <t>3a.Are all core brands on display?</t>
-  </si>
-  <si>
-    <t>WMNH4</t>
-  </si>
-  <si>
-    <t>Question 4:Is there a stand alone still display # 1 ?</t>
-  </si>
-  <si>
-    <t>WMNH5</t>
-  </si>
-  <si>
-    <t>Question 5:Is there a second stand alone Still display?</t>
-  </si>
-  <si>
-    <t>WMNH6</t>
-  </si>
-  <si>
-    <t>Question 6:Are all Coke delivered brands available and ready for sale?  Take a picture and add a comment for each OOS.  Capture all OOS instances in the OOS feature while conducting the survey.</t>
-  </si>
-  <si>
-    <t>WMNH7</t>
-  </si>
-  <si>
-    <t>Question 7:Do we have KO cold availability in self checkoutand/orexpress checkout ?</t>
-  </si>
-  <si>
-    <t>WMNH8</t>
-  </si>
-  <si>
-    <t>Question 8:Is there a Premium SSD display executed in this outlet ?</t>
-  </si>
-  <si>
-    <t>WMNH10</t>
-  </si>
-  <si>
-    <t>Question 10: If there is a Core Can End Cap display in this outlet, is it in first position to our competitors?</t>
-  </si>
-  <si>
-    <t>WMNH11</t>
-  </si>
-  <si>
-    <t>Question 11:Are all displays properly priced?</t>
-  </si>
-  <si>
-    <t>WMNH12</t>
-  </si>
-  <si>
-    <t>Question 12:Do the beverage aisle shelf tag retails match the display retails?</t>
-  </si>
-  <si>
-    <t>WMNH13</t>
-  </si>
-  <si>
-    <t>Question 13:Is all cold equipment properly priced?</t>
-  </si>
-  <si>
-    <t>WMNH14</t>
-  </si>
-  <si>
-    <t>Question 14:Are coolers with our products in the Best position in the checkout area &gt; = primary competition ?</t>
-  </si>
-  <si>
-    <t>WMSC</t>
-  </si>
-  <si>
-    <t>WMSC1</t>
-  </si>
-  <si>
-    <t>Question 1: Is there a SSD 52 week Large Pack End Cap/Display in this outlet ?</t>
-  </si>
-  <si>
-    <t>WMSC1a</t>
-  </si>
-  <si>
-    <t>WMSC2</t>
-  </si>
-  <si>
-    <t>Question 2:Is there a Meal Bundle Display executed in this outlet ?</t>
-  </si>
-  <si>
-    <t>WMSC3</t>
-  </si>
-  <si>
-    <t>Question 3:Is there a SSD Flavor program executed in this outlet ?</t>
-  </si>
-  <si>
-    <t>WMSC4</t>
-  </si>
-  <si>
-    <t>Question 4:Is there a PowerAde multipack display in this outlet ?</t>
-  </si>
-  <si>
-    <t>WMSC5</t>
-  </si>
-  <si>
-    <t>Question 5:Is there an incremental Minican Display in the outlet?  Minimum Display of 6 cases with at least 4 brands on display.</t>
-  </si>
-  <si>
-    <t>WMSC6</t>
-  </si>
-  <si>
-    <t>Question 6:Is there a Monster display in this outlet ?</t>
-  </si>
-  <si>
-    <t>WMSC7</t>
-  </si>
-  <si>
-    <t>Question 7:Is there a Dasani display?</t>
-  </si>
-  <si>
-    <t>WMSC8</t>
-  </si>
-  <si>
-    <t>Question 8:Is there a Gold Peak Tea Rack or Display executed in this outlet ?</t>
-  </si>
-  <si>
-    <t>WMSC9</t>
-  </si>
-  <si>
-    <t>Question 9:Is there a Premium SSD display executed in this outlet ?</t>
-  </si>
-  <si>
-    <t>WMSC10</t>
-  </si>
-  <si>
-    <t>Question 10:Is there cold availability located in the Garden Center area?</t>
-  </si>
-  <si>
-    <t>WMSC12</t>
-  </si>
-  <si>
-    <t>Question 12:Is there a Smartwater display executed in this outlet?</t>
-  </si>
-  <si>
-    <t>WMSC13</t>
-  </si>
-  <si>
-    <t>Question 13:Is there a Monster End Cap with cooler or stand alone cooler in this outlet ?</t>
-  </si>
-  <si>
-    <t>WMSC14</t>
-  </si>
-  <si>
-    <t>Question 14:Is there a Hydrate and Recover Display in this outlet?  Brands must include both PowerAde and Core Power.</t>
-  </si>
-  <si>
-    <t>WMSC15</t>
-  </si>
-  <si>
-    <t>Question 15:Is there a SSD Transaction display executed in this outlet?</t>
-  </si>
-  <si>
-    <t>WMSC16</t>
-  </si>
-  <si>
-    <t>Question 16:Is there a Coffee bin/display/saddlebags executed in this outlet ?</t>
-  </si>
-  <si>
-    <t>WMSC16a</t>
-  </si>
-  <si>
-    <t>16a.Do we have KO cold availability in self checkoutand/orexpress checkout ?</t>
-  </si>
-  <si>
-    <t>WMSC17</t>
-  </si>
-  <si>
-    <t>Question 17:Are all authorized SPK and Still CCBCU products available and ready for sale?  Take a picture and add a comment for each OOS.  Capture all OOS instances in the OOS feature while conducting the survey.</t>
-  </si>
-  <si>
-    <t>WMSC18</t>
-  </si>
-  <si>
-    <t>Question 18:Are all displays properly priced?</t>
-  </si>
-  <si>
-    <t>WMSC19</t>
-  </si>
-  <si>
-    <t>Question 19:Are the beverage aisle shelf tag retails matching display retails?</t>
-  </si>
-  <si>
-    <t>WMSC20</t>
-  </si>
-  <si>
-    <t>Question 20:Are all SKUs in cold door equipment properly priced?</t>
-  </si>
-  <si>
-    <t>WMSC21</t>
-  </si>
-  <si>
-    <t>Question 21:Are coolers with our products in the Best position in the checkout area &gt; = primary competition ?</t>
-  </si>
-  <si>
-    <t>FSOP - Cafeteria</t>
-  </si>
-  <si>
-    <t>Dining1</t>
-  </si>
-  <si>
-    <t>Do we have branded Coca-Cola Cold Drink Equipment in the outlet?  (Fountain, Cooler, Vender, Other = Yes; Dealer Owned non branded = No)</t>
-  </si>
-  <si>
-    <t>Dining2</t>
-  </si>
-  <si>
-    <t>Is our Coca-Cola Cold Drink Equipment in the best position?  (Retail – 1st in traffic flow at the entrance/register.  Eat/Drink – Highest visible location, Easily accessible to consumers to drive awareness)</t>
-  </si>
-  <si>
-    <t>Dining3</t>
-  </si>
-  <si>
-    <t>Is our Coca-Cola Cold Drink Equipment clean, filled, cold and working properly with the lights or translights on?  (May have to open door for lights if EMS sleeping or on timer)</t>
-  </si>
-  <si>
-    <t>Dining4</t>
-  </si>
-  <si>
-    <t>Does equipment contain ONLY Coca-Cola beverage products (purity)?  (Only Coca-Cola/CCR products. No foreign products, food items or water valves.)</t>
-  </si>
-  <si>
-    <t>Dining5</t>
-  </si>
-  <si>
-    <t>Are all Coca-Cola core brands available?  (Coke markets (KO, DK, KOZ, SP,GP, DAS, SW); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS, SW)[Fountain Outlets pass with 4 Core SSD:  KO, DK, KOZ, SP:  Plus DP in DP markets)</t>
-  </si>
-  <si>
-    <t>Dining6</t>
-  </si>
-  <si>
-    <t>Is KO the Exclusive Sparkling Beverage offered in the Outlet?  (Includes all packages, Core Brands, Secondary Brands)</t>
-  </si>
-  <si>
-    <t>Dining7</t>
-  </si>
-  <si>
-    <t>Is KO the Exclusive Still Beverage offered in the Outlet?  (Includes all packages, Core Brands, Secondary Brands) (Includes Energy, Tea, MMJTG)</t>
-  </si>
-  <si>
-    <t>Dining8</t>
-  </si>
-  <si>
-    <t>Is there  Smartwater or Dasani Ambient Water rack placed?  (Includes racks placed individually or on top of an existing cooler)</t>
-  </si>
-  <si>
-    <t>Dining9</t>
-  </si>
-  <si>
-    <t>Is there Coca Cola meal beverage combo available and messaging in the outlet?  (Correct occasion with meal item including Coke Package and Bundle Price)</t>
-  </si>
-  <si>
-    <t>Dining10</t>
-  </si>
-  <si>
-    <t>Have we merchandised the outlet with Occasion Messaging?  (Occasion Messaging: With Food, On the Go Breaktime, Wellness Hydration, On the Go Refreshment (door decal, static cling, counter card, cooler graphics, shelf strip))</t>
-  </si>
-  <si>
-    <t>Dining11</t>
-  </si>
-  <si>
-    <t>Additional Cooler placement (Premium, Energy, Breakfast, Innovation)?  (Counter Top or Impulse Cooler)</t>
-  </si>
-  <si>
-    <t>Dining12</t>
-  </si>
-  <si>
-    <t>Are all Coca-Cola products in date?  (Includes all Bottle / Can and BIB Products)</t>
-  </si>
-  <si>
-    <t>FSOP - Fitness</t>
-  </si>
-  <si>
-    <t>Fitness1</t>
-  </si>
-  <si>
-    <t>Fitness2</t>
-  </si>
-  <si>
-    <t>Fitness3</t>
-  </si>
-  <si>
-    <t>Fitness4</t>
-  </si>
-  <si>
-    <t>Fitness5</t>
-  </si>
-  <si>
-    <t>Are all Coca-Cola core brands available?  (Outlet serves ALL 6  brands (PWRAD, Core Power, DAS, SW, VW, DAS Spk))</t>
-  </si>
-  <si>
-    <t>Fitness6</t>
-  </si>
-  <si>
-    <t>Is KO the Exclusive Still Beverage offered in the Outlet?  (Includes all packages, Core Brands, Secondary Brands)</t>
-  </si>
-  <si>
-    <t>Fitness7</t>
-  </si>
-  <si>
-    <t>Fitness8</t>
-  </si>
-  <si>
-    <t>Have we merchandised the outlet with Occasion Messaging?  (Fitness Hydration messaging (door decal, static cling, counter card, cooler graphics, shelf strip))</t>
-  </si>
-  <si>
-    <t>Fitness9</t>
-  </si>
-  <si>
-    <t>FSOP - Lodging</t>
-  </si>
-  <si>
-    <t>Lodging1</t>
-  </si>
-  <si>
-    <t>Do we have Cold Drink Equipment in the outlet?  (Fountain, Cooler, Vender, Other = Yes; Dealer Owned non branded = Yes)</t>
-  </si>
-  <si>
-    <t>Lodging2</t>
-  </si>
-  <si>
-    <t>Lodging3</t>
-  </si>
-  <si>
-    <t>Lodging4</t>
-  </si>
-  <si>
-    <t>Lodging5</t>
-  </si>
-  <si>
-    <t>Are all Coca-Cola core brands available?  (Coke Markets (KO, DK, KOZ, SP,GP, DAS, SW); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS, SW))</t>
-  </si>
-  <si>
-    <t>Lodging6</t>
-  </si>
-  <si>
-    <t>Lodging7</t>
-  </si>
-  <si>
-    <t>Lodging8</t>
-  </si>
-  <si>
-    <t>Lodging9</t>
-  </si>
-  <si>
-    <t>Is there Coca Cola snack beverage combo available and messaging in the outlet?  [Correct occasion with snack item including Coke Package]</t>
-  </si>
-  <si>
-    <t>Lodging10</t>
-  </si>
-  <si>
-    <t>Have we merchandised the outlet with Occasion Messaging?  (Occasion Messaging: On the Go Refreshment, Wellness Hydration (door decal, static cling, counter card, cooler graphics, shelf strip))</t>
-  </si>
-  <si>
-    <t>Lodging11</t>
-  </si>
-  <si>
-    <t>Is Dasani/Smartwater available in-room or given to guest at Check Inn?  (Includes Neck Ringer on product in room)</t>
-  </si>
-  <si>
-    <t>Lodging12</t>
-  </si>
-  <si>
-    <t>Lodging13</t>
-  </si>
-  <si>
-    <t>FSOP - Transportation</t>
-  </si>
-  <si>
-    <t>Transportation1</t>
-  </si>
-  <si>
-    <t>Transportation2</t>
-  </si>
-  <si>
-    <t>Transportation3</t>
-  </si>
-  <si>
-    <t>Transportation4</t>
-  </si>
-  <si>
-    <t>Transportation5</t>
-  </si>
-  <si>
-    <t>Are all Coca-Cola core brands available?  (Coke markets (KO, DK, KOZ, SP,GP, DAS, SW, Monster); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS, SW, Monster))</t>
-  </si>
-  <si>
-    <t>Transportation6</t>
-  </si>
-  <si>
-    <t>Transportation7</t>
-  </si>
-  <si>
-    <t>Transportation8</t>
-  </si>
-  <si>
-    <t>Transportation9</t>
-  </si>
-  <si>
-    <t>Is there Coca Cola meal and/or snack beverage combo available and messaging in the outlet?  (Correct occasion with meal item including Coke Package and Bundle Price)</t>
-  </si>
-  <si>
-    <t>Transportation10</t>
-  </si>
-  <si>
-    <t>Have we merchandised the outlet with Occasion Messaging?  (Occasion Messaging: On the Go Refreshment, With Food, Wellness Hydration (door decal, static cling, counter card, cooler graphics, shelf strip))</t>
-  </si>
-  <si>
-    <t>Transportation11</t>
-  </si>
-  <si>
-    <t>Transportation12</t>
-  </si>
-  <si>
-    <t>FSOP - Amusement Rec</t>
-  </si>
-  <si>
-    <t>Amusement1</t>
-  </si>
-  <si>
-    <t>Amusement2</t>
-  </si>
-  <si>
-    <t>Amusement3</t>
-  </si>
-  <si>
-    <t>Amusement4</t>
-  </si>
-  <si>
-    <t>Amusement5</t>
-  </si>
-  <si>
-    <t>Are all Coca-Cola core brands available?  (Coke markets (KO, DK, KOZ, SP,GP, DAS, SW); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS, SW))</t>
-  </si>
-  <si>
-    <t>Amusement6</t>
-  </si>
-  <si>
-    <t>Amusement7</t>
-  </si>
-  <si>
-    <t>Amusement8</t>
-  </si>
-  <si>
-    <t>Amusement9</t>
-  </si>
-  <si>
-    <t>Is there Coca Cola meal/snack beverage combo available and messaging in the outlet?  [Correct occasion with meal/snack item including Coke Package and Bundle Price ]</t>
-  </si>
-  <si>
-    <t>Amusement10</t>
-  </si>
-  <si>
-    <t>Amusement11</t>
-  </si>
-  <si>
-    <t>Amusement12</t>
-  </si>
-  <si>
-    <t>FSOP - Specality Retail</t>
-  </si>
-  <si>
-    <t>SpecRetail1</t>
-  </si>
-  <si>
-    <t>SpecRetail2</t>
-  </si>
-  <si>
-    <t>SpecRetail3</t>
-  </si>
-  <si>
-    <t>SpecRetail4</t>
-  </si>
-  <si>
-    <t>SpecRetail5</t>
-  </si>
-  <si>
-    <t>SpecRetail6</t>
-  </si>
-  <si>
-    <t>SpecRetail7</t>
-  </si>
-  <si>
-    <t>SpecRetail8</t>
-  </si>
-  <si>
-    <t>SpecRetail9</t>
-  </si>
-  <si>
-    <t>SpecRetail10</t>
-  </si>
-  <si>
-    <t>Have we merchandised the outlet with Occasion Messaging?  (Occasion Messaging: On the Go Refreshment, Wellness Hydration, Fitness Hydration (door decal, static cling, counter card, cooler graphics, shelf strip))</t>
-  </si>
-  <si>
-    <t>SpecRetail11</t>
-  </si>
-  <si>
-    <t>Additional Cooler placement (Premium, Energy, Innovation)?  (Counter Top or Impulse Cooler)</t>
-  </si>
-  <si>
-    <t>SpecRetail12</t>
-  </si>
-  <si>
-    <t>FSOP - Micro Mart</t>
-  </si>
-  <si>
-    <t>CURetail1</t>
-  </si>
-  <si>
-    <t>CURetail2</t>
-  </si>
-  <si>
-    <t>CURetail3</t>
-  </si>
-  <si>
-    <t>CURetail4</t>
-  </si>
-  <si>
-    <t>CURetail5</t>
-  </si>
-  <si>
-    <t>Are all Coca-Cola core brands available?  (Coke Markets (KO, DK, KOZ, SP,GP, DAS, SW, Monster); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS, SW, Monster))</t>
-  </si>
-  <si>
-    <t>CURetail6</t>
-  </si>
-  <si>
-    <t>CURetail7</t>
-  </si>
-  <si>
-    <t>CURetail8</t>
-  </si>
-  <si>
-    <t>CURetail9</t>
-  </si>
-  <si>
-    <t>Is there Coca Cola Snack beverage combo available and messaging in the outlet?  [Correct occasion with snack item including Coke Package]</t>
-  </si>
-  <si>
-    <t>CURetail10</t>
-  </si>
-  <si>
-    <t>Have we merchandised the outlet with Occasion Messaging?  (Occasion Messaging: On the Go Refreshment, On the Go Breaktime, With Food, Wellness Hydration (door decal, static cling, counter card, cooler graphics, shelf strip))</t>
-  </si>
-  <si>
-    <t>CURetail11</t>
-  </si>
-  <si>
-    <t>Additional Cooler placement (Premium, Energy, Breakfast, Innovation)?  (Counter Top or Impulse cooler)</t>
-  </si>
-  <si>
-    <t>CURetail12</t>
-  </si>
-  <si>
-    <t>FSOP - Restaurant</t>
-  </si>
-  <si>
-    <t>Restaurant1</t>
-  </si>
-  <si>
-    <t>Restaurant3</t>
-  </si>
-  <si>
-    <t>Restaurant4</t>
-  </si>
-  <si>
-    <t>Restaurant5</t>
-  </si>
-  <si>
-    <t>Are all Coca-Cola core brands available?  (Coke markets (KO, DK, KOZ, SP,GP, DAS or SW); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS or SW); [Fountain Outlets pass with 4 Core SSD:  KO, DK, KOZ, SP:  Plus DP in DP markets)</t>
-  </si>
-  <si>
-    <t>Restaurant6</t>
-  </si>
-  <si>
-    <t>Restaurant7</t>
-  </si>
-  <si>
-    <t>Is KO the Exclusive Still Beverage offered in the Outlet?  (Includes all packages, Core Brands, Secondary Brands) (Restaurant must have at a minimum: GPT (Brewed or B/C), Bottled Water (Dasani or SW))</t>
-  </si>
-  <si>
-    <t>Restaurant12</t>
-  </si>
-  <si>
-    <t>FSOP - Vending</t>
-  </si>
-  <si>
-    <t>Vending1</t>
-  </si>
-  <si>
-    <t>Is equipment operational?  (Test buttons to be sure that pricing shows in LED screen. Answer YES if everything is in working condition. May ask customers whether equipment is operational in certain cases such as vending equipment. Verify if payment systems are working (DBV light flashing, Card reader lights flashing, correct change light off, out of stock light off). Vending banks - all equipment must be working)</t>
-  </si>
-  <si>
-    <t>Vending2</t>
-  </si>
-  <si>
-    <t>All product instock in the vender?  (All brands/product in the vender must be instock.  No empty columns.  Vending banks - all venders must be without an out of stock product.)</t>
-  </si>
-  <si>
-    <t>Vending3</t>
-  </si>
-  <si>
-    <t>Core Brands + Dasani available in core SPK vender?  (Are all Coca-Cola core brands available?  Coca-Cola markets: KO, DKO and/or KOZ, SP, GP, DAS.  Dr Pepper markets: include Dr Pepper as a core brand.  If can vender, Gold Peak will not be available. If vender(s) are at secondary schools, the vender(s) comply with USDA guidelines.)</t>
-  </si>
-  <si>
-    <t>Vending4</t>
-  </si>
-  <si>
-    <t>Is service sticker with service phone # on vender?  (If there sticker is present and the telephone number is legible.  Sticker must be on all venders in a vending bank. The Service Sticker must have  the CCBCU Customer Service telephone number,   and asset number legible.  Stickers must be on all venders in a vending bank.)</t>
-  </si>
-  <si>
-    <t>Vending5</t>
-  </si>
-  <si>
-    <t>Vend strips most current logo (W/Calorie Count)?  (Surveyor will check to ensure all logos are the most current available (With Calorie Count). Surveyor will answer yes if all are current. Surveyor will answer no if one or more are not the most current available. N/A if vender is a Glass Front.  Vend strips must be correct on all venders in a vending bank.)</t>
-  </si>
-  <si>
-    <t>Vending6</t>
-  </si>
-  <si>
-    <t>Is package &amp; price clearly comm other than LED?  (If the vender has a price posted for the consumer other than the price displayed on the LED readout.  Package and pricing must be communicated on all venders in a vending bank.)</t>
-  </si>
-  <si>
-    <t>Vending7</t>
-  </si>
-  <si>
-    <t>Is Vend Front appropriate for the consumer occasion?  (If the vend front branding is appropriate - should be sparkling in most instances, but for example in schools, need to be Zero brands or in Fitness should be still branded.   All venders in a vending bank must have occasion appropriate messaging.)</t>
-  </si>
-  <si>
-    <t>Vending8</t>
-  </si>
-  <si>
-    <t>Does the vender meet CCBCU image standards?  (Vend-front, buttons, marketing panel, vend strips must be clear, clean, and not faded. Vender must be functioning and vending product properly. NO graffiti and other unauthorized signage present (signs posted by the public, etc) NO obvious signs of damage or disrepair which distracting from the image of the trademark or functionality of the unit. All venders considered in bank.)</t>
-  </si>
-  <si>
-    <t>Vending9</t>
-  </si>
-  <si>
-    <t>Clear on Calories Messaging present?  (If clear on calories messaging is present somewhere on the vender (example: sticker on top right corner).  All venders in a vending bank must contain "Clear on Calorie" messaging.)</t>
-  </si>
-  <si>
-    <t>Vending10</t>
-  </si>
-  <si>
-    <t>Is appropriate merchandising in place?  (Ad panel cards or snipes with consumer brand info are present. Ad panel can be a cashless message, a Local Theme or Brand Message other than vend front.    If Cashless is available, cashless POS communicates the ability to accept all cashless options.   (Refer to merchandising standards))</t>
-  </si>
-  <si>
-    <t>Vending11</t>
-  </si>
-  <si>
-    <t>Are we Winning at the Outlet?  (The vender(s) are in first/best position.  The venders have more share of space than our competitors.  The vender(s) are competitively priced.  The Customer is satisfied with our service.)</t>
-  </si>
-  <si>
-    <t>QSR</t>
-  </si>
-  <si>
-    <t>QSR1</t>
-  </si>
-  <si>
-    <t>QSR2</t>
-  </si>
-  <si>
-    <t>QSR3</t>
-  </si>
-  <si>
-    <t>QSR4</t>
-  </si>
-  <si>
-    <t>QSR5</t>
-  </si>
-  <si>
-    <t>Are all Coca-Cola core brands available?  (Coke markets (KO, DK, KOZ, SP,GP, DAS); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS); [Fountain Outlets pass with 4 Core SSD:  KO, DK, KOZ, SP:  Plus DP in DP markets)</t>
-  </si>
-  <si>
-    <t>QSR6</t>
-  </si>
-  <si>
-    <t>QSR7</t>
-  </si>
-  <si>
-    <t>QSR8</t>
-  </si>
-  <si>
-    <t>QSR9</t>
-  </si>
-  <si>
-    <t>QSR10</t>
-  </si>
-  <si>
-    <t>Have we merchandised the outlet with our LOS Execution and Occasion Messaging?  (PUSH/PULL, COMBO BOARD, TABLE TENTS, COUNTER  MESSAGING, Occasion Messaging: With Food  (static cling, cooler graphics, shelf strip)</t>
-  </si>
-  <si>
-    <t>QSR11</t>
-  </si>
-  <si>
-    <t>QSR12</t>
-  </si>
-  <si>
-    <t>Name in PRESALE</t>
-  </si>
-  <si>
-    <t>question_text</t>
-  </si>
-  <si>
-    <t>question_ID</t>
-  </si>
-  <si>
-    <t>accepted_answer</t>
-  </si>
-  <si>
-    <t>required_answer</t>
-  </si>
-  <si>
-    <t>PICOS POI # 1:  Do we have a Coke branded cooler in the Impulse Zone?   (The Impulse Zone is within 12 ft. of the register.  Electric Barrel coolers are acceptable. Ice Barrels do NOT count for Impulse Zone but do count for innovation brands in POI # 11. Must be incremental cooler placement, Cold Vault or Cold vault extension does not count.  )</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>1a.  Are ANY of the following 2018 Innovation Brands available in Impulse Zone area? (Coke Origins, Diet Coke Recast, Fanta Apple, VW Active, Core Power Coffee, Fuze 16.9 oz, Powerade Blue Rasp. Cherry, New Dasani Sparkling Flavors, Hubert's Lemonade, McCafe, MM Watermelon, New Dunkin Flavors, Monster Ultra Violet, Gold Peak Unsweet Rasp, Gold Peak Slight Sweet Lemon, Honest Tea Glass, Zico Jalapeno Mango)</t>
-  </si>
-  <si>
-    <t>1aa.  Are ANY of the following 2018 Innovation Brands available? (Coke Origins, Diet Coke Recast, Fanta Apple, VW Active, Core Power Coffee, Fuze 16.9 oz, Powerade Blue Rasp. Cherry, New Dasani Sparkling Flavors, Hubert's Lemonade, McCafe, MM Watermelon, New Dunkin Flavors, Monster Ultra Violet, Gold Peak Unsweet Rasp, Gold Peak Slight Sweet Lemon, Honest Tea Glass, Zico Jalapeno Mango)</t>
-  </si>
-  <si>
-    <t>1b.  Are all the 20oz SSD core brands plus Dasani 20oz represented in the Impulse Zone cooler?  (Core brands are Coke, Coke Zero Sugar, Diet Coke, Sprite, Dr Pepper [where distributed] and Dasani 20oz. )</t>
-  </si>
-  <si>
-    <t>PICOS POI # 2:  Is there a Sparkling can display?</t>
-  </si>
-  <si>
-    <t>2a. Are all core brands on display? (SSD core brands must be present.  Coke, Coke Zero Sugar, Diet Coke, Sprite and Dr Pepper (where distributed).  Any multipack SSD FC can product configuration is acceptable.  )</t>
-  </si>
-  <si>
-    <t>2b.  Is Dasani 12pk 12oz on display?</t>
-  </si>
-  <si>
-    <t>PICOS POI # 3:  Is there a Powerade Display in this outlet (any pkg)?</t>
-  </si>
-  <si>
-    <t>PICOS POI # 4:  Is there an incremental Branded (Monster, NOS or Full Throttle graphics) Energy Cooler in this outlet? (Incremental to the impulse zone cooler, Monster JAVA coolers do not count.  Monster JAVA coolers count in the Coffee POI # 8.)</t>
-  </si>
-  <si>
-    <t>PICOS POI # 5:  Is there a Sparkling PET display? (SSD core brands must be present [Coke, Coke Zero Sugar, Diet Coke, Sprite and Dr Pepper (where distributed)].  Any PET SSD FC PET product configuration is acceptable.  2 Liter, 1.25 Liter  count.  )</t>
-  </si>
-  <si>
-    <t>5a. Are all core brands on display?</t>
-  </si>
-  <si>
-    <t>PICOS POI #6: Is there a Still Display excluding Dasani Casepack Water in this outlet? (Display types could be an end cap, stand alone/free standing, rack or wing.  If displayed with other categories, it would still count toward this question. Incremental to 12pk 12oz Dasani on SSD Display.  Categories could include Energy, Tea, Sports, Water (excluding case pack water), TEY.)</t>
-  </si>
-  <si>
-    <t>PICOS POI # 7:  Is there an incremental SmartWater Display or Rack in this outlet? (Must be incremental to Still Display #1.)</t>
-  </si>
-  <si>
-    <t>PICOS POI # 8:  Is there a Branded Coffee Cooler in this outlet ? (Options include :  Dunkin Donuts, Monster Java, McCafe.  "Breakfast Center" Branding counts.)</t>
-  </si>
-  <si>
-    <t>PICOS POI # 9:  Do we have a Coke branded barrel, ice chest or incremental Coke identified cooler (cold availability) in the outlet? (Barrel and / or incremental cooler can have any branded SSD or Still logo.  Barrel and / or cooler must be incremental to Impulse Zone cooler.  Incremental cooler cannot be an extension of the cold vault.)</t>
-  </si>
-  <si>
-    <t>PICOS POI # 10:  Is there a Coke Identified Fountain in this outlet with pricing POS available (never on logo panel)?</t>
-  </si>
-  <si>
-    <t>PICOS POI # 11:  Is Gold Peak brewed tea, brewed coffee or tea tower available in this outlet?</t>
-  </si>
-  <si>
-    <t>12. Are there any Out of Stock Products in the Outlet? (Base OOS determination on POG and/or shelf tags. One SKU of any package or brand would result in an OOS.)</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>13: Is there a Premium SSD package offered cold in the outlet (8oz, 12oz glass, 8.5 oz aluminum or Import glass)? (Package must be cold not ambient)</t>
-  </si>
-  <si>
-    <t>14: Are there 5 flavors of Gold Peak 18.5oz "cold" available in this outlet?</t>
-  </si>
-  <si>
-    <t>15: Are there 5 flavors of Fanta 20oz "cold" available in this outlet?</t>
-  </si>
-  <si>
-    <t>16: Are there 2+ packages of SmartWater available in this outlet? (Includes cold vault and stand alone displays.)</t>
-  </si>
-  <si>
-    <t>17: Are there 2+ packages of Dasani available in this outlet? (Includes cold vault and stand alone displays.)</t>
-  </si>
-  <si>
-    <t>18:  Is Sparkling Can display in best position?</t>
-  </si>
-  <si>
-    <t>19:  Is Sparkling PET display in best position?</t>
-  </si>
-  <si>
-    <t>20: Is Still Display (excluding Dasani Casepack Water) in best position?</t>
-  </si>
-  <si>
-    <t>21: PICOS POI -  Is the KO SSD messaging "Taste the Feeling" for sparkling IC core brand package visible from the outside?  SSD IC Pkg./Price will vary. 
+    <t xml:space="preserve">Region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group_target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incremental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNITED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 1:Do we have a Coke branded cooler in the Impulse Zone?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1a.Is 2018 Innovation available in the Impulse Zone area, either in an FLM or ice barrel?”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT1b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1b.Are all the 20oz SSD core brands plus Dasani 20oz represented in the Impulse Zone cooler?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 2:Is there a Sparkling can display?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2a.Are all core brands on display?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT2b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2b.Is Dasani 12pk 12oz on display?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 3:Is there a Powerade Display in this outlet (any pkg)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 4:Is there an incrementalBranded (Monster, NOS or Full Throttle graphics) Energy Coolerin this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 5:Is there a Sparkling PET display?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT5a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5a.Are all core brands on display?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI #6:Is there a Still Displayexcluding Dasani Casepack Waterin this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 7:Is there an incremental SmartWater Display or Rack in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 8:Is there a Branded Coffee Cooler in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 9:Do we have a Coke branded barrel, ice chest or incremental Coke identified cooler (cold availability) in the outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 10:Is there a Coke Identified Fountain in this outlet with pricing POS available (never on logo panel)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 11:Is Gold Peak brewed tea, brewed coffee or tea tower available in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:Are all authorized SPK and Still CCBCU products available and ready for sale?  Take a picture and add a comment for each OOS. Capture all OOS instances in the OOS feature while conducting the survey.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:Is there a Premium SSD package offered cold in the outlet (8oz, 12oz glass, 8.5 oz aluminum or Import glass)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:Are there 5 flavors of Gold Peak 18.5oz"cold"available in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:Are there 5 flavors of Fanta 20oz"cold"available in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:Are there 2+ packages of SmartWater available in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:Are there 2+ packages of Dasani available in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:Is Sparkling Can display in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19:Is Sparkling PET display in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20:Is Still Display(excluding Dasani Casepack Water)in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21: PICOS POI -Is the KO SSD messaging "Taste the Feeling" for sparkling IC core brand package visible from the outside?SSD IC Pkg./Price will vary.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:Are there a minimum 5 SSD POIfrom curb to cold vault?("Taste the Feeling" for sparkling IC core brand package)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23: PICOS POI -Is there aFood Solutionwith SSD in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24:Are Coca-Cola identified fountain cups available in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25: PICOS POI -Are there a minimum 3 Monster POIs from curb to cold vault?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26:Are all displays properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR&amp;LT27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27:Are all SKUs in cold vault/equipment properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:Is there a Coke SSD FEM / FLM in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1a:Do we have a Coke cooler in checkout area of the outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug1b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1b:Are all the 20oz SSD core brands plus Dasani 20oz represented in the cooler?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug1c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1c:Is the FLM cooler and cold vault space if available priced correctly?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:Is there a SmartWater Rack incremental tofirststill display in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:Is there a free standing ambient water rack in or around the pharmacy?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:Is there a Transaction Package Display present in the store?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5:Is there a Still Display in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:Is there a Sparkling Display in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug6a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6a.Are all core brands available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:Are the Gold Peak multipack or Gold Peak 64 oz or Honest Tea 59 oz available in the warm section?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:Is Dasani Sparkling available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:Are Dasani 20oz &amp; 1 Liter available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:Is Powerade 4 pk. 20 oz or 6pk 12oz available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:Are 4 SKUs of Dunkin or McCafe available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:If there is a Coke SSD FEM/FLM in this outlet, is it in first position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14. If there is a Sparkling display in this outlet, is it in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.Are all displays properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOSPOI # 1:Sparkling Display #1: Is there a SSD display in this outlet?  SSD Transaction Package must be included.  Still is optional.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1a.Is there a SSD transaction package co-merchandised?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket1b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1b.Are all core brands available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOSPOI # 2:Still HydrationDisplay # 1 (Include Water and/or PowerAde).Is there a Hydration Still display that includes water and/orPowerade?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2a. If a Water Display Is Dasani sparkling co-merchandised or if Sports Display is PowerAde multi-pack co-merchandised?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOSPOI # 3:Sparkling Display #2: Is there a SSD display in this outlet?SSD Transaction Package must be included.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket3a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3a.Does display include SSD transaction packages?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket3b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3b.Are all core brands available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI #4.Do we have KO cold availability in self checkoutand/orexpress checkout ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket4a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4a.Is 20oz KO Sparkling and Dasani available in all 20 oz FLM coolers ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 5 :Is there an incremental Minican Display in the outlet?  Minimum Display of 6 cases with at least 4 brands on display.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOSPOI # 6:Still HydrationDisplay # 2 (Include Water and/or PowerAde).Is there a Hydration Still display that includes water and/orPowerade?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket6a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6a. If a Water Display Is Dasani Sparkling co-merchandised or if Sports Display is PowerAde multi-pack co-merchandised?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 7:Is there an incremental Sparkling non Cola or Flavor Display in this outlet?Brand Options include:  Fanta / Sprite / Mello Yello / Barqs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 8:Is there a SmartWaterRackor Display incremental to Hydration displays #1 &amp; #2 in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOSPOI # 9:Is there a Meal Combo with SSD and Gold Peak Tea executed in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOSPOI # 10:Is there a Coca-Cola Sparkling with a SnackBundlein this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOSPOI # 11:Is there aGold Peak Tearack/display in the outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 12:Is there an Energy (Monster, Full Throttle or NOS) Display or Cooler executed in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 13  Is there a Coffee Display, Rack or Cooler executed in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOSPOI # 14:Is there an incremental Premium SSD package display or rack in the outlet (8oz glass,12 oz 4pk, 12oz 6pk,8.5oz aluminum or Import glass) ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 15:Is there a Dasani Sparkling water display in this outlet?  Display must include at least 4 flavors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 16:  Is there a Hydrate and Recover Display in this outlet?  Brands must include both PowerAde and Core Power.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.Are all authorized SPK and Still CCBCU products available and ready for sale?  Take a picture and add a comment for each OOS. Capture all OOS instances in the OOS feature while conducting the survey.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.Are all displays properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.Are all SKUs in cold door equipment properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20:Are the beverage aisle shelf tag retails matching display retails?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.Is there an SSD display in quad 1?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.Is SSD display in quad 1 in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.Is Still Hydration display #1 in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.Are Front-End FLM /Coolers with our products in the Best position in the checkout area &gt; = primary competition?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1a.Are Monster Energy products available in Coke FEM / FLM?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2: If there is a Sparkling display in this outlet, is display in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2a.Are all core brands available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:Is there a Transactional Pkg Sparkling Display in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:Is there a Sparkling Flavor Future Consumption Display in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:Are all authorized SPK and Still CCBCU products available and ready for sale?  Take a picture and add a comment for each OOS.  Capture all OOS instances in the OOS feature while conducting the survey.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:Are Monster Multipacks available in the warm set?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:Is Gold Peak 18.5oz available in the Still Section?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:Is SmartWater 1 Liter and/or 700 ml available in the Still Section?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:Are Dasani 20oz &amp; 1 Liter available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:Is Powerade 4pk. 20oz or 6pk 12oz available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:Are two SKUs of McCafe available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.If there is a Sparkling display in this outlet, is display in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.Are all displays properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.Are all beverage aisle SKUs properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.All cold equipment properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 1: Is there a Core Can End Cap/Display in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1a.Are all core brands available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 2:Is there a SSD Flavor program executed in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 3:Is  there an SSD display in the outlet with one of the following transaction packages; (mini-cans, 6pk 500ml, 8pk 12oz)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH3a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3a.Are all core brands on display?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 4:Is there a stand alone still display # 1 ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 5:Is there a second stand alone Still display?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 6:Are all Coke delivered brands available and ready for sale?  Take a picture and add a comment for each OOS.  Capture all OOS instances in the OOS feature while conducting the survey.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 7:Do we have KO cold availability in self checkoutand/orexpress checkout ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 8:Is there a Premium SSD display executed in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 10: If there is a Core Can End Cap display in this outlet, is it in first position to our competitors?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 11:Are all displays properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 12:Do the beverage aisle shelf tag retails match the display retails?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 13:Is all cold equipment properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMNH14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 14:Are coolers with our products in the Best position in the checkout area &gt; = primary competition ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 1: Is there a SSD 52 week Large Pack End Cap/Display in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 2:Is there a Meal Bundle Display executed in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 3:Is there a SSD Flavor program executed in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 4:Is there a PowerAde multipack display in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 5:Is there an incremental Minican Display in the outlet?  Minimum Display of 6 cases with at least 4 brands on display.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 6:Is there a Monster display in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 7:Is there a Dasani display?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 8:Is there a Gold Peak Tea Rack or Display executed in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 9:Is there a Premium SSD display executed in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 10:Is there cold availability located in the Garden Center area?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 12:Is there a Smartwater display executed in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 13:Is there a Monster End Cap with cooler or stand alone cooler in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 14:Is there a Hydrate and Recover Display in this outlet?  Brands must include both PowerAde and Core Power.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 15:Is there a SSD Transaction display executed in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 16:Is there a Coffee bin/display/saddlebags executed in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC16a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16a.Do we have KO cold availability in self checkoutand/orexpress checkout ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 17:Are all authorized SPK and Still CCBCU products available and ready for sale?  Take a picture and add a comment for each OOS.  Capture all OOS instances in the OOS feature while conducting the survey.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 18:Are all displays properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 19:Are the beverage aisle shelf tag retails matching display retails?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 20:Are all SKUs in cold door equipment properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WMSC21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 21:Are coolers with our products in the Best position in the checkout area &gt; = primary competition ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSOP - Cafeteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dining1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do we have branded Coca-Cola Cold Drink Equipment in the outlet?  (Fountain, Cooler, Vender, Other = Yes; Dealer Owned non branded = No)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dining2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is our Coca-Cola Cold Drink Equipment in the best position?  (Retail – 1st in traffic flow at the entrance/register.  Eat/Drink – Highest visible location, Easily accessible to consumers to drive awareness)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dining3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is our Coca-Cola Cold Drink Equipment clean, filled, cold and working properly with the lights or translights on?  (May have to open door for lights if EMS sleeping or on timer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dining4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does equipment contain ONLY Coca-Cola beverage products (purity)?  (Only Coca-Cola/CCR products. No foreign products, food items or water valves.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dining5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are all Coca-Cola core brands available?  (Coke markets (KO, DK, KOZ, SP,GP, DAS, SW); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS, SW)[Fountain Outlets pass with 4 Core SSD:  KO, DK, KOZ, SP:  Plus DP in DP markets)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dining6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is KO the Exclusive Sparkling Beverage offered in the Outlet?  (Includes all packages, Core Brands, Secondary Brands)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dining7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is KO the Exclusive Still Beverage offered in the Outlet?  (Includes all packages, Core Brands, Secondary Brands) (Includes Energy, Tea, MMJTG)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dining8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there  Smartwater or Dasani Ambient Water rack placed?  (Includes racks placed individually or on top of an existing cooler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dining9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there Coca Cola meal beverage combo available and messaging in the outlet?  (Correct occasion with meal item including Coke Package and Bundle Price)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dining10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have we merchandised the outlet with Occasion Messaging?  (Occasion Messaging: With Food, On the Go Breaktime, Wellness Hydration, On the Go Refreshment (door decal, static cling, counter card, cooler graphics, shelf strip))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dining11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Cooler placement (Premium, Energy, Breakfast, Innovation)?  (Counter Top or Impulse Cooler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dining12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are all Coca-Cola products in date?  (Includes all Bottle / Can and BIB Products)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSOP - Fitness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fitness1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fitness2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fitness3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fitness4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fitness5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are all Coca-Cola core brands available?  (Outlet serves ALL 6  brands (PWRAD, Core Power, DAS, SW, VW, DAS Spk))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fitness6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is KO the Exclusive Still Beverage offered in the Outlet?  (Includes all packages, Core Brands, Secondary Brands)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fitness7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fitness8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have we merchandised the outlet with Occasion Messaging?  (Fitness Hydration messaging (door decal, static cling, counter card, cooler graphics, shelf strip))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fitness9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSOP - Lodging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do we have Cold Drink Equipment in the outlet?  (Fountain, Cooler, Vender, Other = Yes; Dealer Owned non branded = Yes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are all Coca-Cola core brands available?  (Coke Markets (KO, DK, KOZ, SP,GP, DAS, SW); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS, SW))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there Coca Cola snack beverage combo available and messaging in the outlet?  [Correct occasion with snack item including Coke Package]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have we merchandised the outlet with Occasion Messaging?  (Occasion Messaging: On the Go Refreshment, Wellness Hydration (door decal, static cling, counter card, cooler graphics, shelf strip))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is Dasani/Smartwater available in-room or given to guest at Check Inn?  (Includes Neck Ringer on product in room)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lodging13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSOP - Transportation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are all Coca-Cola core brands available?  (Coke markets (KO, DK, KOZ, SP,GP, DAS, SW, Monster); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS, SW, Monster))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there Coca Cola meal and/or snack beverage combo available and messaging in the outlet?  (Correct occasion with meal item including Coke Package and Bundle Price)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have we merchandised the outlet with Occasion Messaging?  (Occasion Messaging: On the Go Refreshment, With Food, Wellness Hydration (door decal, static cling, counter card, cooler graphics, shelf strip))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transportation12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSOP - Amusement Rec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amusement1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amusement2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amusement3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amusement4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amusement5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are all Coca-Cola core brands available?  (Coke markets (KO, DK, KOZ, SP,GP, DAS, SW); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS, SW))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amusement6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amusement7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amusement8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amusement9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there Coca Cola meal/snack beverage combo available and messaging in the outlet?  [Correct occasion with meal/snack item including Coke Package and Bundle Price ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amusement10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amusement11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amusement12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSOP - Specality Retail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecRetail1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecRetail2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecRetail3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecRetail4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecRetail5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecRetail6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecRetail7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecRetail8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecRetail9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecRetail10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have we merchandised the outlet with Occasion Messaging?  (Occasion Messaging: On the Go Refreshment, Wellness Hydration, Fitness Hydration (door decal, static cling, counter card, cooler graphics, shelf strip))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecRetail11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Cooler placement (Premium, Energy, Innovation)?  (Counter Top or Impulse Cooler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecRetail12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSOP - Micro Mart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURetail1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURetail2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURetail3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURetail4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURetail5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are all Coca-Cola core brands available?  (Coke Markets (KO, DK, KOZ, SP,GP, DAS, SW, Monster); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS, SW, Monster))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURetail6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURetail7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURetail8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURetail9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there Coca Cola Snack beverage combo available and messaging in the outlet?  [Correct occasion with snack item including Coke Package]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURetail10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have we merchandised the outlet with Occasion Messaging?  (Occasion Messaging: On the Go Refreshment, On the Go Breaktime, With Food, Wellness Hydration (door decal, static cling, counter card, cooler graphics, shelf strip))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURetail11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Cooler placement (Premium, Energy, Breakfast, Innovation)?  (Counter Top or Impulse cooler)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURetail12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSOP - Restaurant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restaurant1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restaurant3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restaurant4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restaurant5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are all Coca-Cola core brands available?  (Coke markets (KO, DK, KOZ, SP,GP, DAS or SW); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS or SW); [Fountain Outlets pass with 4 Core SSD:  KO, DK, KOZ, SP:  Plus DP in DP markets)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restaurant6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restaurant7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is KO the Exclusive Still Beverage offered in the Outlet?  (Includes all packages, Core Brands, Secondary Brands) (Restaurant must have at a minimum: GPT (Brewed or B/C), Bottled Water (Dasani or SW))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restaurant12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSOP - Vending</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vending1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is equipment operational?  (Test buttons to be sure that pricing shows in LED screen. Answer YES if everything is in working condition. May ask customers whether equipment is operational in certain cases such as vending equipment. Verify if payment systems are working (DBV light flashing, Card reader lights flashing, correct change light off, out of stock light off). Vending banks - all equipment must be working)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vending2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All product instock in the vender?  (All brands/product in the vender must be instock.  No empty columns.  Vending banks - all venders must be without an out of stock product.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vending3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core Brands + Dasani available in core SPK vender?  (Are all Coca-Cola core brands available?  Coca-Cola markets: KO, DKO and/or KOZ, SP, GP, DAS.  Dr Pepper markets: include Dr Pepper as a core brand.  If can vender, Gold Peak will not be available. If vender(s) are at secondary schools, the vender(s) comply with USDA guidelines.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vending4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is service sticker with service phone # on vender?  (If there sticker is present and the telephone number is legible.  Sticker must be on all venders in a vending bank. The Service Sticker must have  the CCBCU Customer Service telephone number,   and asset number legible.  Stickers must be on all venders in a vending bank.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vending5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vend strips most current logo (W/Calorie Count)?  (Surveyor will check to ensure all logos are the most current available (With Calorie Count). Surveyor will answer yes if all are current. Surveyor will answer no if one or more are not the most current available. N/A if vender is a Glass Front.  Vend strips must be correct on all venders in a vending bank.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vending6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is package &amp; price clearly comm other than LED?  (If the vender has a price posted for the consumer other than the price displayed on the LED readout.  Package and pricing must be communicated on all venders in a vending bank.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vending7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is Vend Front appropriate for the consumer occasion?  (If the vend front branding is appropriate - should be sparkling in most instances, but for example in schools, need to be Zero brands or in Fitness should be still branded.   All venders in a vending bank must have occasion appropriate messaging.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vending8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does the vender meet CCBCU image standards?  (Vend-front, buttons, marketing panel, vend strips must be clear, clean, and not faded. Vender must be functioning and vending product properly. NO graffiti and other unauthorized signage present (signs posted by the public, etc) NO obvious signs of damage or disrepair which distracting from the image of the trademark or functionality of the unit. All venders considered in bank.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vending9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear on Calories Messaging present?  (If clear on calories messaging is present somewhere on the vender (example: sticker on top right corner).  All venders in a vending bank must contain "Clear on Calorie" messaging.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vending10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is appropriate merchandising in place?  (Ad panel cards or snipes with consumer brand info are present. Ad panel can be a cashless message, a Local Theme or Brand Message other than vend front.    If Cashless is available, cashless POS communicates the ability to accept all cashless options.   (Refer to merchandising standards))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vending11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are we Winning at the Outlet?  (The vender(s) are in first/best position.  The venders have more share of space than our competitors.  The vender(s) are competitively priced.  The Customer is satisfied with our service.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are all Coca-Cola core brands available?  (Coke markets (KO, DK, KOZ, SP,GP, DAS); Dr Pepper markets (KO, DK, KOZ, SP,DP,GP, DAS); [Fountain Outlets pass with 4 Core SSD:  KO, DK, KOZ, SP:  Plus DP in DP markets)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have we merchandised the outlet with our LOS Execution and Occasion Messaging?  (PUSH/PULL, COMBO BOARD, TABLE TENTS, COUNTER  MESSAGING, Occasion Messaging: With Food  (static cling, cooler graphics, shelf strip)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name in PRESALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">question_text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">question_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accepted_answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">required_answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 1:  Do we have a Coke branded cooler in the Impulse Zone?   (The Impulse Zone is within 12 ft. of the register.  Electric Barrel coolers are acceptable. Ice Barrels do NOT count for Impulse Zone but do count for innovation brands in POI # 11. Must be incremental cooler placement, Cold Vault or Cold vault extension does not count.  )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1a.  Are ANY of the following 2018 Innovation Brands available in Impulse Zone area? (Coke Origins, Diet Coke Recast, Fanta Apple, VW Active, Core Power Coffee, Fuze 16.9 oz, Powerade Blue Rasp. Cherry, New Dasani Sparkling Flavors, Hubert's Lemonade, McCafe, MM Watermelon, New Dunkin Flavors, Monster Ultra Violet, Gold Peak Unsweet Rasp, Gold Peak Slight Sweet Lemon, Honest Tea Glass, Zico Jalapeno Mango)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1aa.  Are ANY of the following 2018 Innovation Brands available? (Coke Origins, Diet Coke Recast, Fanta Apple, VW Active, Core Power Coffee, Fuze 16.9 oz, Powerade Blue Rasp. Cherry, New Dasani Sparkling Flavors, Hubert's Lemonade, McCafe, MM Watermelon, New Dunkin Flavors, Monster Ultra Violet, Gold Peak Unsweet Rasp, Gold Peak Slight Sweet Lemon, Honest Tea Glass, Zico Jalapeno Mango)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1b.  Are all the 20oz SSD core brands plus Dasani 20oz represented in the Impulse Zone cooler?  (Core brands are Coke, Coke Zero Sugar, Diet Coke, Sprite, Dr Pepper [where distributed] and Dasani 20oz. )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 2:  Is there a Sparkling can display?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2a. Are all core brands on display? (SSD core brands must be present.  Coke, Coke Zero Sugar, Diet Coke, Sprite and Dr Pepper (where distributed).  Any multipack SSD FC can product configuration is acceptable.  )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2b.  Is Dasani 12pk 12oz on display?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 3:  Is there a Powerade Display in this outlet (any pkg)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 4:  Is there an incremental Branded (Monster, NOS or Full Throttle graphics) Energy Cooler in this outlet? (Incremental to the impulse zone cooler, Monster JAVA coolers do not count.  Monster JAVA coolers count in the Coffee POI # 8.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 5:  Is there a Sparkling PET display? (SSD core brands must be present [Coke, Coke Zero Sugar, Diet Coke, Sprite and Dr Pepper (where distributed)].  Any PET SSD FC PET product configuration is acceptable.  2 Liter, 1.25 Liter  count.  )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5a. Are all core brands on display?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI #6: Is there a Still Display excluding Dasani Casepack Water in this outlet? (Display types could be an end cap, stand alone/free standing, rack or wing.  If displayed with other categories, it would still count toward this question. Incremental to 12pk 12oz Dasani on SSD Display.  Categories could include Energy, Tea, Sports, Water (excluding case pack water), TEY.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 7:  Is there an incremental SmartWater Display or Rack in this outlet? (Must be incremental to Still Display #1.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 8:  Is there a Branded Coffee Cooler in this outlet ? (Options include :  Dunkin Donuts, Monster Java, McCafe.  "Breakfast Center" Branding counts.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 9:  Do we have a Coke branded barrel, ice chest or incremental Coke identified cooler (cold availability) in the outlet? (Barrel and / or incremental cooler can have any branded SSD or Still logo.  Barrel and / or cooler must be incremental to Impulse Zone cooler.  Incremental cooler cannot be an extension of the cold vault.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 10:  Is there a Coke Identified Fountain in this outlet with pricing POS available (never on logo panel)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 11:  Is Gold Peak brewed tea, brewed coffee or tea tower available in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. Are there any Out of Stock Products in the Outlet? (Base OOS determination on POG and/or shelf tags. One SKU of any package or brand would result in an OOS.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13: Is there a Premium SSD package offered cold in the outlet (8oz, 12oz glass, 8.5 oz aluminum or Import glass)? (Package must be cold not ambient)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14: Are there 5 flavors of Gold Peak 18.5oz "cold" available in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15: Are there 5 flavors of Fanta 20oz "cold" available in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16: Are there 2+ packages of SmartWater available in this outlet? (Includes cold vault and stand alone displays.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17: Are there 2+ packages of Dasani available in this outlet? (Includes cold vault and stand alone displays.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:  Is Sparkling Can display in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19:  Is Sparkling PET display in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20: Is Still Display (excluding Dasani Casepack Water) in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21: PICOS POI -  Is the KO SSD messaging "Taste the Feeling" for sparkling IC core brand package visible from the outside?  SSD IC Pkg./Price will vary. 
  (Messaging may be at curb, pump, or perimeter of store.  Examples include pole signs, bumper shrouds, pump blades, or window posters. )</t>
   </si>
   <si>
-    <t>22: Are there a minimum 5 SSD POI from curb to cold vault?   ("Taste the Feeling" for sparkling IC core brand package) (YES If there are five or more SSD points of contact. Banners/Coroplast-1, Pump Toppers/Gas Pump Signage-1, Push/Pulls/Window Signs-1, POS on a display-1, KO logo Fountain, Cold vault-1, Incremental KO branded cold equipment &gt; POINTS ARE TO BE AWARDED BASED ON ZONE ACTIVATION LISTED ABOVE.)</t>
-  </si>
-  <si>
-    <t>23: PICOS POI -  Is there a Food Solution with SSD in this outlet?  
+    <t xml:space="preserve">22: Are there a minimum 5 SSD POI from curb to cold vault?   ("Taste the Feeling" for sparkling IC core brand package) (YES If there are five or more SSD points of contact. Banners/Coroplast-1, Pump Toppers/Gas Pump Signage-1, Push/Pulls/Window Signs-1, POS on a display-1, KO logo Fountain, Cold vault-1, Incremental KO branded cold equipment &gt; POINTS ARE TO BE AWARDED BASED ON ZONE ACTIVATION LISTED ABOVE.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23: PICOS POI -  Is there a Food Solution with SSD in this outlet?  
  (The meal or salty snack food bundle can be executed in any part of the outlet.  Sugar snacks should NOT be included (i.e. candy bars).  Combo pricing does NOT need to be included in POS to get a "YES".)</t>
   </si>
   <si>
-    <t>24: Are Coca-Cola identified fountain cups available in this outlet?</t>
-  </si>
-  <si>
-    <t>25: PICOS POI - Are there a minimum 3 Monster POIs from curb to cold vault?  (Curb in POI for MONSTER, Minimum of 3 MONSTER POIs.  May include coolers, Displays, POP elements.)</t>
-  </si>
-  <si>
-    <t>26: Are all displays properly priced?</t>
-  </si>
-  <si>
-    <t>27: Are all SKU's in cold vault/equipment properly priced?</t>
-  </si>
-  <si>
-    <t>1: Is there a Coke SSD FEM / FLM in this outlet?</t>
-  </si>
-  <si>
-    <t>1a: Do we have a Coke cooler in checkout area of the outlet? (Within 12' of register. )</t>
-  </si>
-  <si>
-    <t>1b: Are all the 20oz SSD core brands plus Dasani 20oz represented in the cooler?  (SSD core brands must be present; Coke, Coke Zero Sugar, Diet Coke, Sprite, and Dr Pepper (where distributed) to enable a Yes.)</t>
-  </si>
-  <si>
-    <t>1c: Is the FLM cooler and cold vault space if available priced correctly?</t>
-  </si>
-  <si>
-    <t>2: Is there a SmartWater Rack incremental to first still display in this outlet? (Incremental to first still display.)</t>
-  </si>
-  <si>
-    <t>3: Is there a free standing ambient water rack in or around the pharmacy?</t>
-  </si>
-  <si>
-    <t>4: Is there a Transaction Package Display present in the store? (Display can be rack / flex rack / endcap / floor display.  )</t>
-  </si>
-  <si>
-    <t>5: Is there a Still Display in this outlet?</t>
-  </si>
-  <si>
-    <t>6: Is there a Sparkling Display in this outlet? (Any package of SSD Core Brands on display)</t>
-  </si>
-  <si>
-    <t>6a. Are all core brands available?</t>
-  </si>
-  <si>
-    <t>7: Are the Gold Peak multipack or Gold Peak 64 oz or Honest Tea 59 oz available in the warm section?</t>
-  </si>
-  <si>
-    <t>8: Is Dasani Sparkling available? (Warm or cold availability)</t>
-  </si>
-  <si>
-    <t>9: Are Dasani 20oz &amp; 1 Liter available? (Warm or cold availability)</t>
-  </si>
-  <si>
-    <t>10: Is Powerade 4 pk. 20 oz or 6pk 12oz available?</t>
-  </si>
-  <si>
-    <t>11: Are 4 SKU's of Dunkin or McCafe available? (Warm or cold availability)</t>
-  </si>
-  <si>
-    <t>13: If there is a Coke SSD FEM/FLM in this outlet, is it in first position?</t>
-  </si>
-  <si>
-    <t>15. Are all displays properly priced?</t>
-  </si>
-  <si>
-    <t>PICOS POI # 1:  Sparkling Display #1: Is there a SSD display in this outlet?  SSD Transaction Package must be included.  Still is optional. (Packages include:  6 pack 500ml, 8 pack 12 oz,  Premium Glass, 7.5 oz can.)</t>
-  </si>
-  <si>
-    <t>1a. Is there a SSD transaction package co-merchandised? (Packages include:  6 pack 500ml, 8 pack 12 oz, Premium Packages, 6 pack glass, 7.5 oz can)</t>
-  </si>
-  <si>
-    <t>1b. Are all core brands available? (SSD core brands must be present; Coke, Coke Zero Sugar, Diet Coke, Sprite, and Dr Pepper (where distributed) should be present.)</t>
-  </si>
-  <si>
-    <t>PICOS POI # 2: Still Hydration Display # 1 (Include Water and/or PowerAde).  Is there a Hydration Still display that includes water and/or Powerade? (Any Dasani, SmartWater or PowerAde package will count for a "YES". )</t>
-  </si>
-  <si>
-    <t>PICOS POI # 3:  Sparkling Display #2: Is there a SSD display in this outlet?  SSD Transaction Package must be included. (Packages include:  6 pack 500ml, 8 pack 12 oz,  Premium Glass, 7.5 oz can.)</t>
-  </si>
-  <si>
-    <t>3a. Does display include SSD transaction packages? (Packages include:  6 pack 500ml, 8 pack 12 oz, Premium Packages, 6 pack glass, 7.5 oz can)</t>
-  </si>
-  <si>
-    <t>3b. Are all core brands available?</t>
-  </si>
-  <si>
-    <t>PICOS POI #4. Do we have KO cold availability in self checkout and express checkout ?</t>
-  </si>
-  <si>
-    <t>4a. Is 20oz KO Sparkling and Dasani available in all 20 oz FLM coolers ?</t>
-  </si>
-  <si>
-    <t>PICOS POI # 5 : Is there an incremental Minican Display in the outlet?  Minimum Display of 6 cases with at least 4 brands on display. (Minican display must be incremental to POIs #1 and 3.)</t>
-  </si>
-  <si>
-    <t>PICOS POI # 6: Still Hydration Display # 2 (Include Water and/or PowerAde).  Is there a Hydration Still display that includes water and/or Powerade? (ANY Dasani, SmartWater or PowerAde package will count for a "YES".  Must be incremental to Hydration Display #1.)</t>
-  </si>
-  <si>
-    <t>PICOS POI # 7:  Is there an incremental Sparkling non Cola or Flavor Display in this outlet?  Brand Options include:  Fanta / Sprite / Mello Yello / Barqs  (Display must be incremental to all other Sparkling Displays.)</t>
-  </si>
-  <si>
-    <t>PICOS POI # 8:  Is there a SmartWater Rack or Display incremental to Hydration displays #1 &amp; #2 in this outlet?   (SmartWater Display could be Rack, Display or other permanent fixture.  Could be SmartWater or Sparkling SmartWater. )</t>
-  </si>
-  <si>
-    <t>PICOS POI # 9:  Is there a Meal Combo with SSD and Gold Peak Tea executed in this outlet ?   (This Sparkling and Gold Peak Tea display is incremental to Questions 1, 2 and 3.  Messaging must be included and Meal Combo item must be within 12' of display to enable a "YES". Deli location is primary target for Meal Combo execution.)</t>
-  </si>
-  <si>
-    <t>PICOS POI # 10:  Is there a Coca-Cola Sparkling with a Snack Bundle in this outlet? (This sparkling display is incremental to Questions 1, 2 and 3.  Messaging must be included and Snack Combo item must be within 12' of sparkling display to enable a "YES".  Excludes 20 oz in cold equipment)</t>
-  </si>
-  <si>
-    <t>PICOS POI # 11:  Is there a Gold Peak Tea rack/display in the outlet? (Incremental to Hydration Display #1, #2 and Gold Peak Meal Combo.)</t>
-  </si>
-  <si>
-    <t>PICOS POI # 12:  Is there an Energy (Monster, Full Throttle or NOS) Display or Cooler executed in this outlet?</t>
-  </si>
-  <si>
-    <t>PICOS POI # 13  Is there a Coffee Display, Rack or Cooler executed in this outlet?   (Brand Options include:  Dunkin, Java, McCafe)</t>
-  </si>
-  <si>
-    <t>PICOS POI # 14:  Is there an incremental Premium SSD package display or rack in the outlet (8oz glass, 12 oz 4pk, 12oz 6pk, 8.5oz aluminum or Import glass) ?</t>
-  </si>
-  <si>
-    <t>PICOS POI # 15:  Is there a Dasani Sparkling water display in this outlet?  Display must include at least 4 flavors.</t>
-  </si>
-  <si>
-    <t>PICOS POI # 16:  Is there a Hydrate and Recover Display in this outlet?  Brands must include both PowerAde and Core Power. (Incremental to Hydration Display #1, #2.  Brands must include both PowerAde and Core Power.)</t>
-  </si>
-  <si>
-    <t>17. Are there any Out of Stock Products in the Outlet? (Base OOS determination on POG and/or shelf tags. One SKU of any package or brand would result in an OOS.)</t>
-  </si>
-  <si>
-    <t>18. Are all displays properly priced?</t>
-  </si>
-  <si>
-    <t>19.  Are all SKUs in cold door equipment properly priced?</t>
-  </si>
-  <si>
-    <t>20: Are the beverage aisle shelf tag retails matching display retails?</t>
-  </si>
-  <si>
-    <t>21. Is there an SSD display in quad 1? (Quad one is defined as first 25% of outlet.  Additionally, a pallet drop at the entrance (just inside the store)  would count toward an acceptable location. )</t>
-  </si>
-  <si>
-    <t>22. Is SSD display in quad 1 in best position?</t>
-  </si>
-  <si>
-    <t>23. Is Still Hydration display #1 in best position?</t>
-  </si>
-  <si>
-    <t>24.  Are Front-End FLM / Coolers with our products in the Best position in the checkout area &gt; = primary competition? (Coolers with Coke products should be represented in self checkout or express register lanes.  If no self checkout / express registers; KO cooler must be present at an open register.  Objective to be in first, best and open locations. If shared coolers, must have "MARKET SHARE" of space.)</t>
-  </si>
-  <si>
-    <t>1a. Are Monster Energy products available in Coke FEM / FLM?</t>
-  </si>
-  <si>
-    <t>2: Is there a Sparkling Display in this outlet?</t>
-  </si>
-  <si>
-    <t>2a. Are all core brands available? (SSD core brands must be present; Coke, Coke Zero Sugar, Diet Coke, Sprite, and Dr Pepper (where distributed) to enable a Yes.)</t>
-  </si>
-  <si>
-    <t>3: Is there a Transactional Pkg Sparkling Display in this outlet?</t>
-  </si>
-  <si>
-    <t>4:  Is there a Sparkling Flavor Future Consumption Display in this outlet?</t>
-  </si>
-  <si>
-    <t>6. Are there any Out of Stock Products in the Outlet? (Base OOS determination on POG and/or shelf tags. One SKU of any package or brand would result in an OOS.)</t>
-  </si>
-  <si>
-    <t>7: Are Monster Multipacks available in the warm set?</t>
-  </si>
-  <si>
-    <t>8: Is Gold Peak 18.5oz available in the Still Section?</t>
-  </si>
-  <si>
-    <t>9: Is SmartWater 1 Liter and/or 700 ml available in the Still Section?</t>
-  </si>
-  <si>
-    <t>10: Are Dasani 20oz &amp; 1 Liter available?</t>
-  </si>
-  <si>
-    <t>11: Is Powerade 4pk. 20oz or 6pk 12oz available?</t>
-  </si>
-  <si>
-    <t>12: Are two SKU's of McCafe available? (Warm or cold availability)</t>
-  </si>
-  <si>
-    <t>13. If there is a Sparkling display in this outlet, is display in best position?</t>
-  </si>
-  <si>
-    <t>14. Are all displays properly priced?</t>
-  </si>
-  <si>
-    <t>15. Are all beverage aisle SKU's properly priced?</t>
-  </si>
-  <si>
-    <t>16. All cold equipment properly priced?</t>
-  </si>
-  <si>
-    <t>Question 1: Is there a Core Can End Cap/Display in this outlet ?  (A pallet drop or endcap in the store with core SSD flavors. )</t>
-  </si>
-  <si>
-    <t>1a.  Are all core brands available?</t>
-  </si>
-  <si>
-    <t>Question 2: Is there a SSD Flavor program executed in this outlet ? (Must be incremental to SSD display. Display can be stand alone/rack/wing and must be incremental to all other SPK displays.  Brand choices are:  Fanta, Sprite, Barqs or Mello Yello.  Display must be incremental to all other Sparkling Displays.)</t>
-  </si>
-  <si>
-    <t>Question 3:  Is  there an SSD display in the outlet with one of the following transaction packages; (mini-cans, 6pk 500ml, 8pk 12oz)?</t>
-  </si>
-  <si>
-    <t>3a.  Are all core brands on display?</t>
-  </si>
-  <si>
-    <t>Question 4: Is there a stand alone still display # 1 ? (Category displays include : Isotonic, tea, juice, water, energy, coffee and enhanced water.  Drops excluded.  Display can be stand alone/rack/wing.)</t>
-  </si>
-  <si>
-    <t>Question 5: Is there a second stand alone Still display? (Category displays include : Isotonic, tea, juice, water, energy, coffee and enhanced water.  Drops excluded. )</t>
-  </si>
-  <si>
-    <t>Question 7:  Do we have KO cold availability in self checkout and express checkout ?</t>
-  </si>
-  <si>
-    <t>Question 8:  Is there a Premium SSD display executed in this outlet ?  (This display should include at least one of the following  packages: 8oz 6pk, Import singles, Import multipack, or 8.5oz Aluminum.  Display can be stand alone/rack/wing and must be incremental to all other SPK displays.)</t>
-  </si>
-  <si>
-    <t>Question 11: Are all displays properly priced?</t>
-  </si>
-  <si>
-    <t>Question 12: Do the beverage aisle shelf tag retails match the display retails? (Accuracy is defined as denoting the correct retail – EDV (Everyday Value) or promotion.)</t>
-  </si>
-  <si>
-    <t>Question 13: Is all cold equipment properly priced?</t>
-  </si>
-  <si>
-    <t>Question 14: Are coolers with our products in the Best position in the checkout area &gt; = primary competition ? ( Objective is to be in first, best locations. If they are shared coolers do we have our "MARKET SHARE" of space)</t>
-  </si>
-  <si>
-    <t>Question 1: Is there a SSD 52 week Large Pack End Cap/Display in this outlet ?  (SSD core brands must be present; Coke, Coke Zero Sugar, Diet Coke, Sprite, and Dr Pepper (where distributed) should be present. )</t>
-  </si>
-  <si>
-    <t>Question 2: Is there a Meal Bundle Display executed in this outlet ? (Must be incremental to SSD display.  Messaging must be included and meal bundle display must be within 12' of sparkling display to enable a "YES")</t>
-  </si>
-  <si>
-    <t>Question 3: Is there a SSD Flavor program executed in this outlet ? (Must be incremental to SSD display. Display can be standalone/rack/wing and must be incremental to all other SPK displays.  Brand choices are:  Fanta, Sprite, Barqs or Mello Yello.  Display must be incremental to all other Sparkling Displays.)</t>
-  </si>
-  <si>
-    <t>Question 4: Is there a PowerAde multipack display in this outlet ? (Display can be standalone/rack/wing and must be incremental to all other still displays.)</t>
-  </si>
-  <si>
-    <t>Question 5: Is there an incremental Minican Display in the outlet?  Minimum Display of 6 cases with at least 4 brands on display. (Minican display must be incremental to 52 Week Endcap)</t>
-  </si>
-  <si>
-    <t>Question 6: Is there a Monster display in this outlet ? (Display can be standalone/rack/wing and must be incremental to all other still displays.)</t>
-  </si>
-  <si>
-    <t>Question 7: Is there a Dasani display? (ANY Dasani package will count for a "YES".)</t>
-  </si>
-  <si>
-    <t>Question 8:  Is there a Gold Peak Tea Rack or Display executed in this outlet ? (Display can be standalone/rack/wing and must be incremental to all other still displays.)</t>
-  </si>
-  <si>
-    <t>Question 9:  Is there a Premium SSD display executed in this outlet ?  (This display should include at least one of the following  packages: 8oz 6pk, Import singles, Import multipack, or 8.5oz Aluminum.  Display can be standalone/rack/wing and must be incremental to all other SPK displays.)</t>
-  </si>
-  <si>
-    <t>Question 10:  Is there cold availability located in the Garden Center area?</t>
-  </si>
-  <si>
-    <t>Question 12:  Is there a Smartwater display executed in this outlet?  (Display can be stand alone/rack/wing and must be incremental to all other still displays.)</t>
-  </si>
-  <si>
-    <t>Question 13:  Is there a Monster End Cap with cooler or stand alone cooler in this outlet ? (If counting Monster cooler it must be Monster branded/identified. )</t>
-  </si>
-  <si>
-    <t>Question 14:  Is there a Hydrate and Recover Display in this outlet?  Brands must include both PowerAde and Core Power. (Incremental to Hydration Display #1, #2.  Brands must include both PowerAde and Core Power.)</t>
-  </si>
-  <si>
-    <t>Question 15: Is there a SSD Transaction display executed in this outlet? (It can be bundled or a stand alone display.  Can be co-merchandised/stand alone/rack or wing.)</t>
-  </si>
-  <si>
-    <t>Question 16:  Is there a Coffee bin/display/saddlebags executed in this outlet ?</t>
-  </si>
-  <si>
-    <t>16a.  Do we have KO cold availability in self checkout and express checkout ?</t>
-  </si>
-  <si>
-    <t>Question 18: Are all displays properly priced?</t>
-  </si>
-  <si>
-    <t>Question 19:  Are the beverage aisle shelf tag retails matching display retails? (Accuracy is defined as denoting the correct retail – EDV (Everyday Value) or promotion.)</t>
-  </si>
-  <si>
-    <t>Question 20: Are all SKUs in cold door equipment properly priced? (All coolers with multiple categories, brand promotions and multiple price points must be priced appropriatley.)</t>
-  </si>
-  <si>
-    <t>Question 21: Are coolers with our products in the Best position in the checkout area &gt; = primary competition ? ( Objective is to be in first, best locations. If they are shared coolers do we have our "MARKET SHARE" of space)</t>
-  </si>
-  <si>
-    <t>Clear on Calorie's Messaging present?  (If clear on calorie's messaging is present somewhere on the vender (example: sticker on top right corner).  All venders in a vending bank must contain "Clear on Calorie" messaging.)</t>
+    <t xml:space="preserve">24: Are Coca-Cola identified fountain cups available in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25: PICOS POI - Are there a minimum 3 Monster POIs from curb to cold vault?  (Curb in POI for MONSTER, Minimum of 3 MONSTER POIs.  May include coolers, Displays, POP elements.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26: Are all displays properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27: Are all SKU's in cold vault/equipment properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Is there a Coke SSD FEM / FLM in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1a: Do we have a Coke cooler in checkout area of the outlet? (Within 12' of register. )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1b: Are all the 20oz SSD core brands plus Dasani 20oz represented in the cooler?  (SSD core brands must be present; Coke, Coke Zero Sugar, Diet Coke, Sprite, and Dr Pepper (where distributed) to enable a Yes.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1c: Is the FLM cooler and cold vault space if available priced correctly?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2: Is there a SmartWater Rack incremental to first still display in this outlet? (Incremental to first still display.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3: Is there a free standing ambient water rack in or around the pharmacy?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4: Is there a Transaction Package Display present in the store? (Display can be rack / flex rack / endcap / floor display.  )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5: Is there a Still Display in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6: Is there a Sparkling Display in this outlet? (Any package of SSD Core Brands on display)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6a. Are all core brands available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7: Are the Gold Peak multipack or Gold Peak 64 oz or Honest Tea 59 oz available in the warm section?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8: Is Dasani Sparkling available? (Warm or cold availability)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9: Are Dasani 20oz &amp; 1 Liter available? (Warm or cold availability)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10: Is Powerade 4 pk. 20 oz or 6pk 12oz available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11: Are 4 SKU's of Dunkin or McCafe available? (Warm or cold availability)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13: If there is a Coke SSD FEM/FLM in this outlet, is it in first position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15. Are all displays properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 1:  Sparkling Display #1: Is there a SSD display in this outlet?  SSD Transaction Package must be included.  Still is optional. (Packages include:  6 pack 500ml, 8 pack 12 oz,  Premium Glass, 7.5 oz can.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1a. Is there a SSD transaction package co-merchandised? (Packages include:  6 pack 500ml, 8 pack 12 oz, Premium Packages, 6 pack glass, 7.5 oz can)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1b. Are all core brands available? (SSD core brands must be present; Coke, Coke Zero Sugar, Diet Coke, Sprite, and Dr Pepper (where distributed) should be present.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 2: Still Hydration Display # 1 (Include Water and/or PowerAde).  Is there a Hydration Still display that includes water and/or Powerade? (Any Dasani, SmartWater or PowerAde package will count for a "YES". )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 3:  Sparkling Display #2: Is there a SSD display in this outlet?  SSD Transaction Package must be included. (Packages include:  6 pack 500ml, 8 pack 12 oz,  Premium Glass, 7.5 oz can.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3a. Does display include SSD transaction packages? (Packages include:  6 pack 500ml, 8 pack 12 oz, Premium Packages, 6 pack glass, 7.5 oz can)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3b. Are all core brands available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI #4. Do we have KO cold availability in self checkout and express checkout ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4a. Is 20oz KO Sparkling and Dasani available in all 20 oz FLM coolers ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 5 : Is there an incremental Minican Display in the outlet?  Minimum Display of 6 cases with at least 4 brands on display. (Minican display must be incremental to POIs #1 and 3.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 6: Still Hydration Display # 2 (Include Water and/or PowerAde).  Is there a Hydration Still display that includes water and/or Powerade? (ANY Dasani, SmartWater or PowerAde package will count for a "YES".  Must be incremental to Hydration Display #1.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 7:  Is there an incremental Sparkling non Cola or Flavor Display in this outlet?  Brand Options include:  Fanta / Sprite / Mello Yello / Barqs  (Display must be incremental to all other Sparkling Displays.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 8:  Is there a SmartWater Rack or Display incremental to Hydration displays #1 &amp; #2 in this outlet?   (SmartWater Display could be Rack, Display or other permanent fixture.  Could be SmartWater or Sparkling SmartWater. )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 9:  Is there a Meal Combo with SSD and Gold Peak Tea executed in this outlet ?   (This Sparkling and Gold Peak Tea display is incremental to Questions 1, 2 and 3.  Messaging must be included and Meal Combo item must be within 12' of display to enable a "YES". Deli location is primary target for Meal Combo execution.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 10:  Is there a Coca-Cola Sparkling with a Snack Bundle in this outlet? (This sparkling display is incremental to Questions 1, 2 and 3.  Messaging must be included and Snack Combo item must be within 12' of sparkling display to enable a "YES".  Excludes 20 oz in cold equipment)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 11:  Is there a Gold Peak Tea rack/display in the outlet? (Incremental to Hydration Display #1, #2 and Gold Peak Meal Combo.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 12:  Is there an Energy (Monster, Full Throttle or NOS) Display or Cooler executed in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 13  Is there a Coffee Display, Rack or Cooler executed in this outlet?   (Brand Options include:  Dunkin, Java, McCafe)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 14:  Is there an incremental Premium SSD package display or rack in the outlet (8oz glass, 12 oz 4pk, 12oz 6pk, 8.5oz aluminum or Import glass) ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 15:  Is there a Dasani Sparkling water display in this outlet?  Display must include at least 4 flavors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICOS POI # 16:  Is there a Hydrate and Recover Display in this outlet?  Brands must include both PowerAde and Core Power. (Incremental to Hydration Display #1, #2.  Brands must include both PowerAde and Core Power.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17. Are there any Out of Stock Products in the Outlet? (Base OOS determination on POG and/or shelf tags. One SKU of any package or brand would result in an OOS.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18. Are all displays properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.  Are all SKUs in cold door equipment properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20: Are the beverage aisle shelf tag retails matching display retails?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21. Is there an SSD display in quad 1? (Quad one is defined as first 25% of outlet.  Additionally, a pallet drop at the entrance (just inside the store)  would count toward an acceptable location. )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22. Is SSD display in quad 1 in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23. Is Still Hydration display #1 in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.  Are Front-End FLM / Coolers with our products in the Best position in the checkout area &gt; = primary competition? (Coolers with Coke products should be represented in self checkout or express register lanes.  If no self checkout / express registers; KO cooler must be present at an open register.  Objective to be in first, best and open locations. If shared coolers, must have "MARKET SHARE" of space.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1a. Are Monster Energy products available in Coke FEM / FLM?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:Is there a Sparkling Display in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2a. Are all core brands available? (SSD core brands must be present; Coke, Coke Zero Sugar, Diet Coke, Sprite, and Dr Pepper (where distributed) to enable a Yes.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3: Is there a Transactional Pkg Sparkling Display in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:  Is there a Sparkling Flavor Future Consumption Display in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Are there any Out of Stock Products in the Outlet? (Base OOS determination on POG and/or shelf tags. One SKU of any package or brand would result in an OOS.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7: Are Monster Multipacks available in the warm set?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8: Is Gold Peak 18.5oz available in the Still Section?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9: Is SmartWater 1 Liter and/or 700 ml available in the Still Section?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10: Are Dasani 20oz &amp; 1 Liter available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11: Is Powerade 4pk. 20oz or 6pk 12oz available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12: Are two SKU's of McCafe available? (Warm or cold availability)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13. If there is a Sparkling display in this outlet, is display in best position?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14. Are all displays properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15. Are all beverage aisle SKU's properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16. All cold equipment properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 1: Is there a Core Can End Cap/Display in this outlet ?  (A pallet drop or endcap in the store with core SSD flavors. )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1a.  Are all core brands available?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 2: Is there a SSD Flavor program executed in this outlet ? (Must be incremental to SSD display. Display can be stand alone/rack/wing and must be incremental to all other SPK displays.  Brand choices are:  Fanta, Sprite, Barqs or Mello Yello.  Display must be incremental to all other Sparkling Displays.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 3:  Is  there an SSD display in the outlet with one of the following transaction packages; (mini-cans, 6pk 500ml, 8pk 12oz)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3a.  Are all core brands on display?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 4: Is there a stand alone still display # 1 ? (Category displays include : Isotonic, tea, juice, water, energy, coffee and enhanced water.  Drops excluded.  Display can be stand alone/rack/wing.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 5: Is there a second stand alone Still display? (Category displays include : Isotonic, tea, juice, water, energy, coffee and enhanced water.  Drops excluded. )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 7:  Do we have KO cold availability in self checkout and express checkout ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 8:  Is there a Premium SSD display executed in this outlet ?  (This display should include at least one of the following  packages: 8oz 6pk, Import singles, Import multipack, or 8.5oz Aluminum.  Display can be stand alone/rack/wing and must be incremental to all other SPK displays.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 11: Are all displays properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 12: Do the beverage aisle shelf tag retails match the display retails? (Accuracy is defined as denoting the correct retail – EDV (Everyday Value) or promotion.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 13: Is all cold equipment properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 14: Are coolers with our products in the Best position in the checkout area &gt; = primary competition ? ( Objective is to be in first, best locations. If they are shared coolers do we have our "MARKET SHARE" of space)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 1: Is there a SSD 52 week Large Pack End Cap/Display in this outlet ?  (SSD core brands must be present; Coke, Coke Zero Sugar, Diet Coke, Sprite, and Dr Pepper (where distributed) should be present. )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 2: Is there a Meal Bundle Display executed in this outlet ? (Must be incremental to SSD display.  Messaging must be included and meal bundle display must be within 12' of sparkling display to enable a "YES")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 3: Is there a SSD Flavor program executed in this outlet ? (Must be incremental to SSD display. Display can be standalone/rack/wing and must be incremental to all other SPK displays.  Brand choices are:  Fanta, Sprite, Barqs or Mello Yello.  Display must be incremental to all other Sparkling Displays.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 4: Is there a PowerAde multipack display in this outlet ? (Display can be standalone/rack/wing and must be incremental to all other still displays.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 5: Is there an incremental Minican Display in the outlet?  Minimum Display of 6 cases with at least 4 brands on display. (Minican display must be incremental to 52 Week Endcap)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 6: Is there a Monster display in this outlet ? (Display can be standalone/rack/wing and must be incremental to all other still displays.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 7: Is there a Dasani display? (ANY Dasani package will count for a "YES".)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 8:  Is there a Gold Peak Tea Rack or Display executed in this outlet ? (Display can be standalone/rack/wing and must be incremental to all other still displays.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 9:  Is there a Premium SSD display executed in this outlet ?  (This display should include at least one of the following  packages: 8oz 6pk, Import singles, Import multipack, or 8.5oz Aluminum.  Display can be standalone/rack/wing and must be incremental to all other SPK displays.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 10:  Is there cold availability located in the Garden Center area?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 12:  Is there a Smartwater display executed in this outlet?  (Display can be stand alone/rack/wing and must be incremental to all other still displays.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 13:  Is there a Monster End Cap with cooler or stand alone cooler in this outlet ? (If counting Monster cooler it must be Monster branded/identified. )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 14:  Is there a Hydrate and Recover Display in this outlet?  Brands must include both PowerAde and Core Power. (Incremental to Hydration Display #1, #2.  Brands must include both PowerAde and Core Power.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 15: Is there a SSD Transaction display executed in this outlet? (It can be bundled or a stand alone display.  Can be co-merchandised/stand alone/rack or wing.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 16:  Is there a Coffee bin/display/saddlebags executed in this outlet ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16a.  Do we have KO cold availability in self checkout and express checkout ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 18: Are all displays properly priced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 19:  Are the beverage aisle shelf tag retails matching display retails? (Accuracy is defined as denoting the correct retail – EDV (Everyday Value) or promotion.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 20: Are all SKUs in cold door equipment properly priced? (All coolers with multiple categories, brand promotions and multiple price points must be priced appropriatley.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question 21: Are coolers with our products in the Best position in the checkout area &gt; = primary competition ? ( Objective is to be in first, best locations. If they are shared coolers do we have our "MARKET SHARE" of space)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear on Calorie's Messaging present?  (If clear on calorie's messaging is present somewhere on the vender (example: sticker on top right corner).  All venders in a vending bank must contain "Clear on Calorie" messaging.)</t>
   </si>
 </sst>
 </file>
@@ -1800,7 +1800,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="9">
@@ -2102,18 +2102,19 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A225" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C227" activeCellId="0" sqref="C227"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A80" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K94" activeCellId="0" sqref="K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.4898785425101"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.8097165991903"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.9878542510121"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4022,7 +4023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="s">
         <v>8</v>
       </c>
@@ -7661,15 +7662,15 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A122" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A129" activeCellId="0" sqref="A129"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A84" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C88" activeCellId="0" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.0202429149798"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.6599190283401"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -9060,10 +9061,10 @@
         <v>179</v>
       </c>
       <c r="B87" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="C87" s="12" t="s">
         <v>180</v>
-      </c>
-      <c r="C87" s="12" t="s">
-        <v>540</v>
       </c>
       <c r="D87" s="18"/>
       <c r="E87" s="10" t="s">

</xml_diff>

<commit_message>
ccbottlersus fix survey Value2
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/Data/SurveyTemplateV2.xlsx
+++ b/Projects/CCBOTTLERSUS/Data/SurveyTemplateV2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="590">
   <si>
     <t xml:space="preserve">Region</t>
   </si>
@@ -1649,6 +1649,9 @@
   </si>
   <si>
     <t xml:space="preserve">2:Is there a Sparkling Display in this outlet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2: Is there a Sparkling Display in this outlet?</t>
   </si>
   <si>
     <t xml:space="preserve">2a. Are all core brands available? (SSD core brands must be present; Coke, Coke Zero Sugar, Diet Coke, Sprite, and Dr Pepper (where distributed) to enable a Yes.)</t>
@@ -2109,11 +2112,11 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.8097165991903"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.2388663967611"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.9878542510121"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -7663,14 +7666,14 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A84" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C88" activeCellId="0" sqref="C88"/>
+      <selection pane="topLeft" activeCell="C89" activeCellId="0" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.6599190283401"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="75.3036437246964"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -9074,10 +9077,10 @@
     </row>
     <row r="88" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>182</v>
+        <v>540</v>
       </c>
       <c r="C88" s="12" t="s">
         <v>541</v>
@@ -9090,10 +9093,10 @@
     </row>
     <row r="89" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>542</v>
@@ -9104,12 +9107,12 @@
       </c>
       <c r="F89" s="10"/>
     </row>
-    <row r="90" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>543</v>
@@ -9120,15 +9123,15 @@
       </c>
       <c r="F90" s="10"/>
     </row>
-    <row r="91" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>90</v>
+        <v>186</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>500</v>
+        <v>544</v>
       </c>
       <c r="D91" s="18"/>
       <c r="E91" s="10" t="s">
@@ -9136,44 +9139,44 @@
       </c>
       <c r="F91" s="10"/>
     </row>
-    <row r="92" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C92" s="11" t="s">
-        <v>544</v>
+        <v>90</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>500</v>
       </c>
       <c r="D92" s="18"/>
       <c r="E92" s="10" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="F92" s="10"/>
     </row>
-    <row r="93" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C93" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C93" s="11" t="s">
         <v>545</v>
       </c>
       <c r="D93" s="18"/>
       <c r="E93" s="10" t="s">
-        <v>459</v>
+        <v>477</v>
       </c>
       <c r="F93" s="10"/>
     </row>
     <row r="94" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C94" s="12" t="s">
         <v>546</v>
@@ -9184,12 +9187,12 @@
       </c>
       <c r="F94" s="10"/>
     </row>
-    <row r="95" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>547</v>
@@ -9200,12 +9203,12 @@
       </c>
       <c r="F95" s="10"/>
     </row>
-    <row r="96" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>548</v>
@@ -9218,10 +9221,10 @@
     </row>
     <row r="97" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C97" s="12" t="s">
         <v>549</v>
@@ -9234,10 +9237,10 @@
     </row>
     <row r="98" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C98" s="12" t="s">
         <v>550</v>
@@ -9248,12 +9251,12 @@
       </c>
       <c r="F98" s="10"/>
     </row>
-    <row r="99" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C99" s="12" t="s">
         <v>551</v>
@@ -9264,12 +9267,12 @@
       </c>
       <c r="F99" s="10"/>
     </row>
-    <row r="100" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C100" s="12" t="s">
         <v>552</v>
@@ -9282,10 +9285,10 @@
     </row>
     <row r="101" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>553</v>
@@ -9298,10 +9301,10 @@
     </row>
     <row r="102" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C102" s="12" t="s">
         <v>554</v>
@@ -9314,10 +9317,10 @@
     </row>
     <row r="103" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C103" s="12" t="s">
         <v>555</v>
@@ -9328,12 +9331,12 @@
       </c>
       <c r="F103" s="10"/>
     </row>
-    <row r="104" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C104" s="12" t="s">
         <v>556</v>
@@ -9344,12 +9347,12 @@
       </c>
       <c r="F104" s="10"/>
     </row>
-    <row r="105" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C105" s="12" t="s">
         <v>557</v>
@@ -9360,12 +9363,12 @@
       </c>
       <c r="F105" s="10"/>
     </row>
-    <row r="106" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>558</v>
@@ -9376,12 +9379,12 @@
       </c>
       <c r="F106" s="10"/>
     </row>
-    <row r="107" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C107" s="12" t="s">
         <v>559</v>
@@ -9392,12 +9395,12 @@
       </c>
       <c r="F107" s="10"/>
     </row>
-    <row r="108" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C108" s="12" t="s">
         <v>560</v>
@@ -9408,12 +9411,12 @@
       </c>
       <c r="F108" s="10"/>
     </row>
-    <row r="109" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C109" s="12" t="s">
         <v>561</v>
@@ -9424,44 +9427,44 @@
       </c>
       <c r="F109" s="10"/>
     </row>
-    <row r="110" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="C110" s="11" t="s">
-        <v>544</v>
+        <v>224</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>562</v>
       </c>
       <c r="D110" s="18"/>
       <c r="E110" s="10" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="F110" s="10"/>
     </row>
-    <row r="111" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="C111" s="12" t="s">
-        <v>562</v>
+        <v>226</v>
+      </c>
+      <c r="C111" s="11" t="s">
+        <v>545</v>
       </c>
       <c r="D111" s="18"/>
       <c r="E111" s="10" t="s">
-        <v>459</v>
+        <v>477</v>
       </c>
       <c r="F111" s="10"/>
     </row>
     <row r="112" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C112" s="12" t="s">
         <v>563</v>
@@ -9474,13 +9477,13 @@
     </row>
     <row r="113" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>232</v>
+        <v>564</v>
       </c>
       <c r="D113" s="18"/>
       <c r="E113" s="10" t="s">
@@ -9488,15 +9491,15 @@
       </c>
       <c r="F113" s="10"/>
     </row>
-    <row r="114" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>564</v>
+        <v>232</v>
       </c>
       <c r="D114" s="18"/>
       <c r="E114" s="10" t="s">
@@ -9504,12 +9507,12 @@
       </c>
       <c r="F114" s="10"/>
     </row>
-    <row r="115" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C115" s="12" t="s">
         <v>565</v>
@@ -9520,12 +9523,12 @@
       </c>
       <c r="F115" s="10"/>
     </row>
-    <row r="116" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C116" s="12" t="s">
         <v>566</v>
@@ -9536,12 +9539,12 @@
       </c>
       <c r="F116" s="10"/>
     </row>
-    <row r="117" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C117" s="12" t="s">
         <v>567</v>
@@ -9552,12 +9555,12 @@
       </c>
       <c r="F117" s="10"/>
     </row>
-    <row r="118" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C118" s="12" t="s">
         <v>568</v>
@@ -9568,15 +9571,15 @@
       </c>
       <c r="F118" s="10"/>
     </row>
-    <row r="119" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>556</v>
+        <v>569</v>
       </c>
       <c r="D119" s="18"/>
       <c r="E119" s="10" t="s">
@@ -9584,15 +9587,15 @@
       </c>
       <c r="F119" s="10"/>
     </row>
-    <row r="120" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>246</v>
+        <v>214</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>569</v>
+        <v>557</v>
       </c>
       <c r="D120" s="18"/>
       <c r="E120" s="10" t="s">
@@ -9600,12 +9603,12 @@
       </c>
       <c r="F120" s="10"/>
     </row>
-    <row r="121" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C121" s="12" t="s">
         <v>570</v>
@@ -9616,12 +9619,12 @@
       </c>
       <c r="F121" s="10"/>
     </row>
-    <row r="122" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C122" s="12" t="s">
         <v>571</v>
@@ -9632,12 +9635,12 @@
       </c>
       <c r="F122" s="10"/>
     </row>
-    <row r="123" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C123" s="12" t="s">
         <v>572</v>
@@ -9648,12 +9651,12 @@
       </c>
       <c r="F123" s="10"/>
     </row>
-    <row r="124" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C124" s="12" t="s">
         <v>573</v>
@@ -9666,10 +9669,10 @@
     </row>
     <row r="125" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C125" s="12" t="s">
         <v>574</v>
@@ -9680,12 +9683,12 @@
       </c>
       <c r="F125" s="10"/>
     </row>
-    <row r="126" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C126" s="12" t="s">
         <v>575</v>
@@ -9696,12 +9699,12 @@
       </c>
       <c r="F126" s="10"/>
     </row>
-    <row r="127" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C127" s="12" t="s">
         <v>576</v>
@@ -9712,12 +9715,12 @@
       </c>
       <c r="F127" s="10"/>
     </row>
-    <row r="128" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C128" s="12" t="s">
         <v>577</v>
@@ -9730,10 +9733,10 @@
     </row>
     <row r="129" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C129" s="12" t="s">
         <v>578</v>
@@ -9746,10 +9749,10 @@
     </row>
     <row r="130" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C130" s="12" t="s">
         <v>579</v>
@@ -9760,12 +9763,12 @@
       </c>
       <c r="F130" s="10"/>
     </row>
-    <row r="131" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C131" s="12" t="s">
         <v>580</v>
@@ -9776,12 +9779,12 @@
       </c>
       <c r="F131" s="10"/>
     </row>
-    <row r="132" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C132" s="12" t="s">
         <v>581</v>
@@ -9794,10 +9797,10 @@
     </row>
     <row r="133" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C133" s="12" t="s">
         <v>582</v>
@@ -9808,12 +9811,12 @@
       </c>
       <c r="F133" s="10"/>
     </row>
-    <row r="134" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C134" s="12" t="s">
         <v>583</v>
@@ -9824,44 +9827,44 @@
       </c>
       <c r="F134" s="10"/>
     </row>
-    <row r="135" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C135" s="11" t="s">
-        <v>531</v>
+        <v>274</v>
+      </c>
+      <c r="C135" s="12" t="s">
+        <v>584</v>
       </c>
       <c r="D135" s="18"/>
       <c r="E135" s="10" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="F135" s="10"/>
     </row>
-    <row r="136" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="C136" s="12" t="s">
-        <v>584</v>
+        <v>276</v>
+      </c>
+      <c r="C136" s="11" t="s">
+        <v>531</v>
       </c>
       <c r="D136" s="18"/>
       <c r="E136" s="10" t="s">
-        <v>459</v>
+        <v>477</v>
       </c>
       <c r="F136" s="10"/>
     </row>
-    <row r="137" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C137" s="12" t="s">
         <v>585</v>
@@ -9874,12 +9877,12 @@
     </row>
     <row r="138" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="C138" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C138" s="12" t="s">
         <v>586</v>
       </c>
       <c r="D138" s="18"/>
@@ -9888,14 +9891,14 @@
       </c>
       <c r="F138" s="10"/>
     </row>
-    <row r="139" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="C139" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C139" s="14" t="s">
         <v>587</v>
       </c>
       <c r="D139" s="18"/>
@@ -9904,15 +9907,15 @@
       </c>
       <c r="F139" s="10"/>
     </row>
-    <row r="140" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="B140" s="11" t="s">
-        <v>287</v>
-      </c>
-      <c r="C140" s="11" t="s">
-        <v>287</v>
+    <row r="140" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C140" s="12" t="s">
+        <v>588</v>
       </c>
       <c r="D140" s="18"/>
       <c r="E140" s="10" t="s">
@@ -9920,15 +9923,15 @@
       </c>
       <c r="F140" s="10"/>
     </row>
-    <row r="141" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C141" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D141" s="18"/>
       <c r="E141" s="10" t="s">
@@ -9936,15 +9939,15 @@
       </c>
       <c r="F141" s="10"/>
     </row>
-    <row r="142" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="10" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B142" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C142" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D142" s="18"/>
       <c r="E142" s="10" t="s">
@@ -9952,15 +9955,15 @@
       </c>
       <c r="F142" s="10"/>
     </row>
-    <row r="143" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D143" s="18"/>
       <c r="E143" s="10" t="s">
@@ -9968,15 +9971,15 @@
       </c>
       <c r="F143" s="10"/>
     </row>
-    <row r="144" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B144" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C144" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D144" s="18"/>
       <c r="E144" s="10" t="s">
@@ -9984,15 +9987,15 @@
       </c>
       <c r="F144" s="10"/>
     </row>
-    <row r="145" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B145" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C145" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D145" s="18"/>
       <c r="E145" s="10" t="s">
@@ -10000,15 +10003,15 @@
       </c>
       <c r="F145" s="10"/>
     </row>
-    <row r="146" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C146" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D146" s="18"/>
       <c r="E146" s="10" t="s">
@@ -10018,13 +10021,13 @@
     </row>
     <row r="147" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C147" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D147" s="18"/>
       <c r="E147" s="10" t="s">
@@ -10034,13 +10037,13 @@
     </row>
     <row r="148" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="10" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B148" s="11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C148" s="11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D148" s="18"/>
       <c r="E148" s="10" t="s">
@@ -10048,15 +10051,15 @@
       </c>
       <c r="F148" s="10"/>
     </row>
-    <row r="149" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="10" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B149" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D149" s="18"/>
       <c r="E149" s="10" t="s">
@@ -10064,15 +10067,15 @@
       </c>
       <c r="F149" s="10"/>
     </row>
-    <row r="150" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B150" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C150" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D150" s="18"/>
       <c r="E150" s="10" t="s">
@@ -10080,15 +10083,15 @@
       </c>
       <c r="F150" s="10"/>
     </row>
-    <row r="151" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B151" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C151" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D151" s="18"/>
       <c r="E151" s="10" t="s">
@@ -10096,15 +10099,15 @@
       </c>
       <c r="F151" s="10"/>
     </row>
-    <row r="152" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="10" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B152" s="11" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="C152" s="11" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="D152" s="18"/>
       <c r="E152" s="10" t="s">
@@ -10112,15 +10115,15 @@
       </c>
       <c r="F152" s="10"/>
     </row>
-    <row r="153" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B153" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C153" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D153" s="18"/>
       <c r="E153" s="10" t="s">
@@ -10128,15 +10131,15 @@
       </c>
       <c r="F153" s="10"/>
     </row>
-    <row r="154" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B154" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C154" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D154" s="18"/>
       <c r="E154" s="10" t="s">
@@ -10144,15 +10147,15 @@
       </c>
       <c r="F154" s="10"/>
     </row>
-    <row r="155" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B155" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C155" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D155" s="18"/>
       <c r="E155" s="10" t="s">
@@ -10160,15 +10163,15 @@
       </c>
       <c r="F155" s="10"/>
     </row>
-    <row r="156" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="10" t="s">
-        <v>315</v>
-      </c>
-      <c r="B156" s="12" t="s">
-        <v>316</v>
-      </c>
-      <c r="C156" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
+      </c>
+      <c r="B156" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="C156" s="11" t="s">
+        <v>293</v>
       </c>
       <c r="D156" s="18"/>
       <c r="E156" s="10" t="s">
@@ -10178,13 +10181,13 @@
     </row>
     <row r="157" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="10" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B157" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C157" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D157" s="18"/>
       <c r="E157" s="10" t="s">
@@ -10192,15 +10195,15 @@
       </c>
       <c r="F157" s="10"/>
     </row>
-    <row r="158" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="10" t="s">
-        <v>319</v>
-      </c>
-      <c r="B158" s="11" t="s">
-        <v>301</v>
-      </c>
-      <c r="C158" s="11" t="s">
-        <v>301</v>
+        <v>317</v>
+      </c>
+      <c r="B158" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="C158" s="12" t="s">
+        <v>318</v>
       </c>
       <c r="D158" s="18"/>
       <c r="E158" s="10" t="s">
@@ -10210,13 +10213,13 @@
     </row>
     <row r="159" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="10" t="s">
-        <v>320</v>
-      </c>
-      <c r="B159" s="12" t="s">
-        <v>321</v>
-      </c>
-      <c r="C159" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
+      </c>
+      <c r="B159" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="C159" s="11" t="s">
+        <v>301</v>
       </c>
       <c r="D159" s="18"/>
       <c r="E159" s="10" t="s">
@@ -10224,15 +10227,15 @@
       </c>
       <c r="F159" s="10"/>
     </row>
-    <row r="160" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="B160" s="11" t="s">
-        <v>309</v>
-      </c>
-      <c r="C160" s="11" t="s">
-        <v>309</v>
+        <v>320</v>
+      </c>
+      <c r="B160" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="C160" s="12" t="s">
+        <v>321</v>
       </c>
       <c r="D160" s="18"/>
       <c r="E160" s="10" t="s">
@@ -10240,15 +10243,15 @@
       </c>
       <c r="F160" s="10"/>
     </row>
-    <row r="161" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="B161" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="C161" s="12" t="s">
-        <v>325</v>
+        <v>322</v>
+      </c>
+      <c r="B161" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="C161" s="11" t="s">
+        <v>309</v>
       </c>
       <c r="D161" s="18"/>
       <c r="E161" s="10" t="s">
@@ -10256,15 +10259,15 @@
       </c>
       <c r="F161" s="10"/>
     </row>
-    <row r="162" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="B162" s="11" t="s">
-        <v>289</v>
-      </c>
-      <c r="C162" s="11" t="s">
-        <v>289</v>
+        <v>324</v>
+      </c>
+      <c r="B162" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="C162" s="12" t="s">
+        <v>325</v>
       </c>
       <c r="D162" s="18"/>
       <c r="E162" s="10" t="s">
@@ -10272,15 +10275,15 @@
       </c>
       <c r="F162" s="10"/>
     </row>
-    <row r="163" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B163" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C163" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D163" s="18"/>
       <c r="E163" s="10" t="s">
@@ -10288,15 +10291,15 @@
       </c>
       <c r="F163" s="10"/>
     </row>
-    <row r="164" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B164" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C164" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D164" s="18"/>
       <c r="E164" s="10" t="s">
@@ -10306,13 +10309,13 @@
     </row>
     <row r="165" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="B165" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="C165" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
+      </c>
+      <c r="B165" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="C165" s="11" t="s">
+        <v>293</v>
       </c>
       <c r="D165" s="18"/>
       <c r="E165" s="10" t="s">
@@ -10320,15 +10323,15 @@
       </c>
       <c r="F165" s="10"/>
     </row>
-    <row r="166" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="10" t="s">
-        <v>331</v>
-      </c>
-      <c r="B166" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="C166" s="11" t="s">
-        <v>297</v>
+        <v>329</v>
+      </c>
+      <c r="B166" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="C166" s="12" t="s">
+        <v>330</v>
       </c>
       <c r="D166" s="18"/>
       <c r="E166" s="10" t="s">
@@ -10336,15 +10339,15 @@
       </c>
       <c r="F166" s="10"/>
     </row>
-    <row r="167" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B167" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C167" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D167" s="18"/>
       <c r="E167" s="10" t="s">
@@ -10354,13 +10357,13 @@
     </row>
     <row r="168" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B168" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C168" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D168" s="18"/>
       <c r="E168" s="10" t="s">
@@ -10370,13 +10373,13 @@
     </row>
     <row r="169" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B169" s="11" t="s">
-        <v>335</v>
+        <v>301</v>
       </c>
       <c r="C169" s="11" t="s">
-        <v>335</v>
+        <v>301</v>
       </c>
       <c r="D169" s="18"/>
       <c r="E169" s="10" t="s">
@@ -10384,15 +10387,15 @@
       </c>
       <c r="F169" s="10"/>
     </row>
-    <row r="170" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B170" s="11" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C170" s="11" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D170" s="18"/>
       <c r="E170" s="10" t="s">
@@ -10400,15 +10403,15 @@
       </c>
       <c r="F170" s="10"/>
     </row>
-    <row r="171" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="B171" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="C171" s="12" t="s">
-        <v>339</v>
+        <v>336</v>
+      </c>
+      <c r="B171" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="C171" s="11" t="s">
+        <v>337</v>
       </c>
       <c r="D171" s="18"/>
       <c r="E171" s="10" t="s">
@@ -10418,13 +10421,13 @@
     </row>
     <row r="172" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="B172" s="11" t="s">
-        <v>307</v>
-      </c>
-      <c r="C172" s="11" t="s">
-        <v>307</v>
+        <v>338</v>
+      </c>
+      <c r="B172" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="C172" s="12" t="s">
+        <v>339</v>
       </c>
       <c r="D172" s="18"/>
       <c r="E172" s="10" t="s">
@@ -10432,15 +10435,15 @@
       </c>
       <c r="F172" s="10"/>
     </row>
-    <row r="173" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B173" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C173" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D173" s="18"/>
       <c r="E173" s="10" t="s">
@@ -10448,15 +10451,15 @@
       </c>
       <c r="F173" s="10"/>
     </row>
-    <row r="174" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B174" s="11" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="C174" s="11" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="D174" s="18"/>
       <c r="E174" s="10" t="s">
@@ -10464,15 +10467,15 @@
       </c>
       <c r="F174" s="10"/>
     </row>
-    <row r="175" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B175" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C175" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D175" s="18"/>
       <c r="E175" s="10" t="s">
@@ -10480,15 +10483,15 @@
       </c>
       <c r="F175" s="10"/>
     </row>
-    <row r="176" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B176" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C176" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D176" s="18"/>
       <c r="E176" s="10" t="s">
@@ -10496,15 +10499,15 @@
       </c>
       <c r="F176" s="10"/>
     </row>
-    <row r="177" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B177" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C177" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D177" s="18"/>
       <c r="E177" s="10" t="s">
@@ -10512,15 +10515,15 @@
       </c>
       <c r="F177" s="10"/>
     </row>
-    <row r="178" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="B178" s="12" t="s">
-        <v>348</v>
-      </c>
-      <c r="C178" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
+      </c>
+      <c r="B178" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="C178" s="11" t="s">
+        <v>293</v>
       </c>
       <c r="D178" s="18"/>
       <c r="E178" s="10" t="s">
@@ -10528,15 +10531,15 @@
       </c>
       <c r="F178" s="10"/>
     </row>
-    <row r="179" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="B179" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="C179" s="11" t="s">
-        <v>297</v>
+        <v>347</v>
+      </c>
+      <c r="B179" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="C179" s="12" t="s">
+        <v>348</v>
       </c>
       <c r="D179" s="18"/>
       <c r="E179" s="10" t="s">
@@ -10544,15 +10547,15 @@
       </c>
       <c r="F179" s="10"/>
     </row>
-    <row r="180" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B180" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C180" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D180" s="18"/>
       <c r="E180" s="10" t="s">
@@ -10562,13 +10565,13 @@
     </row>
     <row r="181" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B181" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C181" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D181" s="18"/>
       <c r="E181" s="10" t="s">
@@ -10576,15 +10579,15 @@
       </c>
       <c r="F181" s="10"/>
     </row>
-    <row r="182" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B182" s="11" t="s">
-        <v>353</v>
+        <v>301</v>
       </c>
       <c r="C182" s="11" t="s">
-        <v>353</v>
+        <v>301</v>
       </c>
       <c r="D182" s="18"/>
       <c r="E182" s="10" t="s">
@@ -10592,15 +10595,15 @@
       </c>
       <c r="F182" s="10"/>
     </row>
-    <row r="183" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B183" s="11" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C183" s="11" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D183" s="18"/>
       <c r="E183" s="10" t="s">
@@ -10608,15 +10611,15 @@
       </c>
       <c r="F183" s="10"/>
     </row>
-    <row r="184" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="10" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B184" s="11" t="s">
-        <v>307</v>
+        <v>355</v>
       </c>
       <c r="C184" s="11" t="s">
-        <v>307</v>
+        <v>355</v>
       </c>
       <c r="D184" s="18"/>
       <c r="E184" s="10" t="s">
@@ -10624,15 +10627,15 @@
       </c>
       <c r="F184" s="10"/>
     </row>
-    <row r="185" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B185" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C185" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D185" s="18"/>
       <c r="E185" s="10" t="s">
@@ -10640,15 +10643,15 @@
       </c>
       <c r="F185" s="10"/>
     </row>
-    <row r="186" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B186" s="11" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="C186" s="11" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="D186" s="18"/>
       <c r="E186" s="10" t="s">
@@ -10656,15 +10659,15 @@
       </c>
       <c r="F186" s="10"/>
     </row>
-    <row r="187" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B187" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C187" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D187" s="18"/>
       <c r="E187" s="10" t="s">
@@ -10672,15 +10675,15 @@
       </c>
       <c r="F187" s="10"/>
     </row>
-    <row r="188" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B188" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C188" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D188" s="18"/>
       <c r="E188" s="10" t="s">
@@ -10688,15 +10691,15 @@
       </c>
       <c r="F188" s="10"/>
     </row>
-    <row r="189" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="10" t="s">
-        <v>362</v>
-      </c>
-      <c r="B189" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="C189" s="12" t="s">
-        <v>293</v>
+        <v>361</v>
+      </c>
+      <c r="B189" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="C189" s="11" t="s">
+        <v>291</v>
       </c>
       <c r="D189" s="18"/>
       <c r="E189" s="10" t="s">
@@ -10706,13 +10709,13 @@
     </row>
     <row r="190" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B190" s="12" t="s">
-        <v>364</v>
+        <v>293</v>
       </c>
       <c r="C190" s="12" t="s">
-        <v>364</v>
+        <v>293</v>
       </c>
       <c r="D190" s="18"/>
       <c r="E190" s="10" t="s">
@@ -10720,15 +10723,15 @@
       </c>
       <c r="F190" s="10"/>
     </row>
-    <row r="191" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="B191" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="C191" s="11" t="s">
-        <v>297</v>
+        <v>363</v>
+      </c>
+      <c r="B191" s="12" t="s">
+        <v>364</v>
+      </c>
+      <c r="C191" s="12" t="s">
+        <v>364</v>
       </c>
       <c r="D191" s="18"/>
       <c r="E191" s="10" t="s">
@@ -10736,15 +10739,15 @@
       </c>
       <c r="F191" s="10"/>
     </row>
-    <row r="192" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B192" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C192" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D192" s="18"/>
       <c r="E192" s="10" t="s">
@@ -10754,13 +10757,13 @@
     </row>
     <row r="193" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B193" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C193" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D193" s="18"/>
       <c r="E193" s="10" t="s">
@@ -10768,15 +10771,15 @@
       </c>
       <c r="F193" s="10"/>
     </row>
-    <row r="194" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B194" s="11" t="s">
-        <v>369</v>
+        <v>301</v>
       </c>
       <c r="C194" s="11" t="s">
-        <v>369</v>
+        <v>301</v>
       </c>
       <c r="D194" s="18"/>
       <c r="E194" s="10" t="s">
@@ -10784,15 +10787,15 @@
       </c>
       <c r="F194" s="10"/>
     </row>
-    <row r="195" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="B195" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="C195" s="13" t="s">
-        <v>355</v>
+        <v>368</v>
+      </c>
+      <c r="B195" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="C195" s="11" t="s">
+        <v>369</v>
       </c>
       <c r="D195" s="18"/>
       <c r="E195" s="10" t="s">
@@ -10800,15 +10803,15 @@
       </c>
       <c r="F195" s="10"/>
     </row>
-    <row r="196" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="B196" s="11" t="s">
-        <v>307</v>
-      </c>
-      <c r="C196" s="11" t="s">
-        <v>307</v>
+        <v>370</v>
+      </c>
+      <c r="B196" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="C196" s="13" t="s">
+        <v>355</v>
       </c>
       <c r="D196" s="18"/>
       <c r="E196" s="10" t="s">
@@ -10816,15 +10819,15 @@
       </c>
       <c r="F196" s="10"/>
     </row>
-    <row r="197" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B197" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C197" s="11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D197" s="18"/>
       <c r="E197" s="10" t="s">
@@ -10832,15 +10835,15 @@
       </c>
       <c r="F197" s="10"/>
     </row>
-    <row r="198" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="10" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B198" s="11" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="C198" s="11" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="D198" s="18"/>
       <c r="E198" s="10" t="s">
@@ -10848,15 +10851,15 @@
       </c>
       <c r="F198" s="10"/>
     </row>
-    <row r="199" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B199" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C199" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D199" s="18"/>
       <c r="E199" s="10" t="s">
@@ -10864,15 +10867,15 @@
       </c>
       <c r="F199" s="10"/>
     </row>
-    <row r="200" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B200" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C200" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D200" s="18"/>
       <c r="E200" s="10" t="s">
@@ -10880,15 +10883,15 @@
       </c>
       <c r="F200" s="10"/>
     </row>
-    <row r="201" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B201" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C201" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D201" s="18"/>
       <c r="E201" s="10" t="s">
@@ -10896,15 +10899,15 @@
       </c>
       <c r="F201" s="10"/>
     </row>
-    <row r="202" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="B202" s="13" t="s">
-        <v>348</v>
-      </c>
-      <c r="C202" s="13" t="s">
-        <v>348</v>
+        <v>377</v>
+      </c>
+      <c r="B202" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="C202" s="11" t="s">
+        <v>293</v>
       </c>
       <c r="D202" s="18"/>
       <c r="E202" s="10" t="s">
@@ -10912,15 +10915,15 @@
       </c>
       <c r="F202" s="10"/>
     </row>
-    <row r="203" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="10" t="s">
-        <v>379</v>
-      </c>
-      <c r="B203" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="C203" s="11" t="s">
-        <v>297</v>
+        <v>378</v>
+      </c>
+      <c r="B203" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="C203" s="13" t="s">
+        <v>348</v>
       </c>
       <c r="D203" s="18"/>
       <c r="E203" s="10" t="s">
@@ -10928,15 +10931,15 @@
       </c>
       <c r="F203" s="10"/>
     </row>
-    <row r="204" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B204" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C204" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D204" s="18"/>
       <c r="E204" s="10" t="s">
@@ -10946,13 +10949,13 @@
     </row>
     <row r="205" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B205" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C205" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D205" s="18"/>
       <c r="E205" s="10" t="s">
@@ -10962,13 +10965,13 @@
     </row>
     <row r="206" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B206" s="11" t="s">
-        <v>335</v>
+        <v>301</v>
       </c>
       <c r="C206" s="11" t="s">
-        <v>335</v>
+        <v>301</v>
       </c>
       <c r="D206" s="18"/>
       <c r="E206" s="10" t="s">
@@ -10976,15 +10979,15 @@
       </c>
       <c r="F206" s="10"/>
     </row>
-    <row r="207" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B207" s="11" t="s">
-        <v>384</v>
+        <v>335</v>
       </c>
       <c r="C207" s="11" t="s">
-        <v>384</v>
+        <v>335</v>
       </c>
       <c r="D207" s="18"/>
       <c r="E207" s="10" t="s">
@@ -10992,15 +10995,15 @@
       </c>
       <c r="F207" s="10"/>
     </row>
-    <row r="208" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="10" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B208" s="11" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C208" s="11" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D208" s="18"/>
       <c r="E208" s="10" t="s">
@@ -11010,13 +11013,13 @@
     </row>
     <row r="209" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="10" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B209" s="11" t="s">
-        <v>309</v>
+        <v>386</v>
       </c>
       <c r="C209" s="11" t="s">
-        <v>309</v>
+        <v>386</v>
       </c>
       <c r="D209" s="18"/>
       <c r="E209" s="10" t="s">
@@ -11024,15 +11027,15 @@
       </c>
       <c r="F209" s="10"/>
     </row>
-    <row r="210" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="10" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B210" s="11" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="C210" s="11" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="D210" s="18"/>
       <c r="E210" s="10" t="s">
@@ -11040,15 +11043,15 @@
       </c>
       <c r="F210" s="10"/>
     </row>
-    <row r="211" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B211" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C211" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D211" s="18"/>
       <c r="E211" s="10" t="s">
@@ -11056,15 +11059,15 @@
       </c>
       <c r="F211" s="10"/>
     </row>
-    <row r="212" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B212" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C212" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D212" s="18"/>
       <c r="E212" s="10" t="s">
@@ -11072,15 +11075,15 @@
       </c>
       <c r="F212" s="10"/>
     </row>
-    <row r="213" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B213" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C213" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D213" s="18"/>
       <c r="E213" s="10" t="s">
@@ -11088,15 +11091,15 @@
       </c>
       <c r="F213" s="10"/>
     </row>
-    <row r="214" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="10" t="s">
-        <v>393</v>
-      </c>
-      <c r="B214" s="12" t="s">
-        <v>394</v>
-      </c>
-      <c r="C214" s="12" t="s">
-        <v>394</v>
+        <v>392</v>
+      </c>
+      <c r="B214" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="C214" s="11" t="s">
+        <v>293</v>
       </c>
       <c r="D214" s="18"/>
       <c r="E214" s="10" t="s">
@@ -11104,15 +11107,15 @@
       </c>
       <c r="F214" s="10"/>
     </row>
-    <row r="215" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="B215" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="C215" s="11" t="s">
-        <v>297</v>
+        <v>393</v>
+      </c>
+      <c r="B215" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="C215" s="12" t="s">
+        <v>394</v>
       </c>
       <c r="D215" s="18"/>
       <c r="E215" s="10" t="s">
@@ -11120,15 +11123,15 @@
       </c>
       <c r="F215" s="10"/>
     </row>
-    <row r="216" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B216" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C216" s="11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D216" s="18"/>
       <c r="E216" s="10" t="s">
@@ -11138,13 +11141,13 @@
     </row>
     <row r="217" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B217" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C217" s="11" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D217" s="18"/>
       <c r="E217" s="10" t="s">
@@ -11154,13 +11157,13 @@
     </row>
     <row r="218" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="B218" s="12" t="s">
-        <v>399</v>
-      </c>
-      <c r="C218" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
+      </c>
+      <c r="B218" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="C218" s="11" t="s">
+        <v>301</v>
       </c>
       <c r="D218" s="18"/>
       <c r="E218" s="10" t="s">
@@ -11168,15 +11171,15 @@
       </c>
       <c r="F218" s="10"/>
     </row>
-    <row r="219" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="B219" s="11" t="s">
-        <v>401</v>
-      </c>
-      <c r="C219" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
+      </c>
+      <c r="B219" s="12" t="s">
+        <v>399</v>
+      </c>
+      <c r="C219" s="12" t="s">
+        <v>399</v>
       </c>
       <c r="D219" s="18"/>
       <c r="E219" s="10" t="s">
@@ -11184,15 +11187,15 @@
       </c>
       <c r="F219" s="10"/>
     </row>
-    <row r="220" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B220" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C220" s="11" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D220" s="18"/>
       <c r="E220" s="10" t="s">
@@ -11200,15 +11203,15 @@
       </c>
       <c r="F220" s="10"/>
     </row>
-    <row r="221" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="10" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B221" s="11" t="s">
-        <v>309</v>
+        <v>403</v>
       </c>
       <c r="C221" s="11" t="s">
-        <v>309</v>
+        <v>403</v>
       </c>
       <c r="D221" s="18"/>
       <c r="E221" s="10" t="s">
@@ -11216,15 +11219,15 @@
       </c>
       <c r="F221" s="10"/>
     </row>
-    <row r="222" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B222" s="11" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="C222" s="11" t="s">
-        <v>287</v>
+        <v>309</v>
       </c>
       <c r="D222" s="18"/>
       <c r="E222" s="10" t="s">
@@ -11232,15 +11235,15 @@
       </c>
       <c r="F222" s="10"/>
     </row>
-    <row r="223" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="10" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B223" s="11" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C223" s="11" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D223" s="18"/>
       <c r="E223" s="10" t="s">
@@ -11248,15 +11251,15 @@
       </c>
       <c r="F223" s="10"/>
     </row>
-    <row r="224" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B224" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C224" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D224" s="18"/>
       <c r="E224" s="10" t="s">
@@ -11264,15 +11267,15 @@
       </c>
       <c r="F224" s="10"/>
     </row>
-    <row r="225" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B225" s="11" t="s">
-        <v>410</v>
+        <v>293</v>
       </c>
       <c r="C225" s="11" t="s">
-        <v>410</v>
+        <v>293</v>
       </c>
       <c r="D225" s="18"/>
       <c r="E225" s="10" t="s">
@@ -11280,15 +11283,15 @@
       </c>
       <c r="F225" s="10"/>
     </row>
-    <row r="226" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="10" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B226" s="11" t="s">
-        <v>297</v>
+        <v>410</v>
       </c>
       <c r="C226" s="11" t="s">
-        <v>297</v>
+        <v>410</v>
       </c>
       <c r="D226" s="18"/>
       <c r="E226" s="10" t="s">
@@ -11296,15 +11299,15 @@
       </c>
       <c r="F226" s="10"/>
     </row>
-    <row r="227" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B227" s="11" t="s">
-        <v>413</v>
+        <v>297</v>
       </c>
       <c r="C227" s="11" t="s">
-        <v>413</v>
+        <v>297</v>
       </c>
       <c r="D227" s="18"/>
       <c r="E227" s="10" t="s">
@@ -11312,15 +11315,15 @@
       </c>
       <c r="F227" s="10"/>
     </row>
-    <row r="228" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="10" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B228" s="11" t="s">
-        <v>309</v>
+        <v>413</v>
       </c>
       <c r="C228" s="11" t="s">
-        <v>309</v>
+        <v>413</v>
       </c>
       <c r="D228" s="18"/>
       <c r="E228" s="10" t="s">
@@ -11328,15 +11331,15 @@
       </c>
       <c r="F228" s="10"/>
     </row>
-    <row r="229" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="10" t="s">
-        <v>416</v>
-      </c>
-      <c r="B229" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="C229" s="14" t="s">
-        <v>417</v>
+        <v>414</v>
+      </c>
+      <c r="B229" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="C229" s="11" t="s">
+        <v>309</v>
       </c>
       <c r="D229" s="18"/>
       <c r="E229" s="10" t="s">
@@ -11344,15 +11347,15 @@
       </c>
       <c r="F229" s="10"/>
     </row>
-    <row r="230" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="10" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B230" s="14" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C230" s="14" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D230" s="18"/>
       <c r="E230" s="10" t="s">
@@ -11360,15 +11363,15 @@
       </c>
       <c r="F230" s="10"/>
     </row>
-    <row r="231" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="10" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B231" s="14" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C231" s="14" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D231" s="18"/>
       <c r="E231" s="10" t="s">
@@ -11378,13 +11381,13 @@
     </row>
     <row r="232" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B232" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C232" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D232" s="18"/>
       <c r="E232" s="10" t="s">
@@ -11392,15 +11395,15 @@
       </c>
       <c r="F232" s="10"/>
     </row>
-    <row r="233" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="B233" s="6" t="s">
-        <v>425</v>
-      </c>
-      <c r="C233" s="6" t="s">
-        <v>425</v>
+    <row r="233" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="B233" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="C233" s="14" t="s">
+        <v>423</v>
       </c>
       <c r="D233" s="18"/>
       <c r="E233" s="10" t="s">
@@ -11408,15 +11411,15 @@
       </c>
       <c r="F233" s="10"/>
     </row>
-    <row r="234" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="B234" s="14" t="s">
-        <v>427</v>
-      </c>
-      <c r="C234" s="14" t="s">
-        <v>427</v>
+    <row r="234" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B234" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="C234" s="6" t="s">
+        <v>425</v>
       </c>
       <c r="D234" s="18"/>
       <c r="E234" s="10" t="s">
@@ -11424,15 +11427,15 @@
       </c>
       <c r="F234" s="10"/>
     </row>
-    <row r="235" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B235" s="14" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C235" s="14" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D235" s="18"/>
       <c r="E235" s="10" t="s">
@@ -11440,15 +11443,15 @@
       </c>
       <c r="F235" s="10"/>
     </row>
-    <row r="236" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B236" s="14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C236" s="14" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D236" s="18"/>
       <c r="E236" s="10" t="s">
@@ -11456,15 +11459,15 @@
       </c>
       <c r="F236" s="10"/>
     </row>
-    <row r="237" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="10" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B237" s="14" t="s">
-        <v>588</v>
+        <v>431</v>
       </c>
       <c r="C237" s="14" t="s">
-        <v>588</v>
+        <v>431</v>
       </c>
       <c r="D237" s="18"/>
       <c r="E237" s="10" t="s">
@@ -11472,15 +11475,15 @@
       </c>
       <c r="F237" s="10"/>
     </row>
-    <row r="238" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="10" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B238" s="14" t="s">
-        <v>435</v>
+        <v>589</v>
       </c>
       <c r="C238" s="14" t="s">
-        <v>435</v>
+        <v>589</v>
       </c>
       <c r="D238" s="18"/>
       <c r="E238" s="10" t="s">
@@ -11488,15 +11491,15 @@
       </c>
       <c r="F238" s="10"/>
     </row>
-    <row r="239" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="10" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B239" s="14" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C239" s="14" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D239" s="18"/>
       <c r="E239" s="10" t="s">
@@ -11504,34 +11507,39 @@
       </c>
       <c r="F239" s="10"/>
     </row>
-    <row r="240" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="13" t="s">
+    <row r="240" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="B240" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="C240" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="D240" s="18"/>
+      <c r="E240" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="F240" s="10"/>
+    </row>
+    <row r="241" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="13" t="s">
         <v>439</v>
       </c>
-      <c r="C240" s="13" t="s">
+      <c r="C241" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="E240" s="10" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="241" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="13" t="s">
+      <c r="E241" s="10" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="13" t="s">
         <v>440</v>
       </c>
-      <c r="C241" s="13" t="s">
+      <c r="C242" s="13" t="s">
         <v>289</v>
-      </c>
-      <c r="E241" s="10" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="242" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="13" t="s">
-        <v>441</v>
-      </c>
-      <c r="C242" s="13" t="s">
-        <v>291</v>
       </c>
       <c r="E242" s="10" t="s">
         <v>459</v>
@@ -11539,32 +11547,32 @@
     </row>
     <row r="243" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="C243" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="E243" s="10" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="C243" s="13" t="s">
+      <c r="C244" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="E243" s="10" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="244" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="13" t="s">
+      <c r="E244" s="10" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="13" t="s">
         <v>443</v>
       </c>
-      <c r="C244" s="13" t="s">
+      <c r="C245" s="13" t="s">
         <v>444</v>
-      </c>
-      <c r="E244" s="10" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="245" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="13" t="s">
-        <v>445</v>
-      </c>
-      <c r="C245" s="13" t="s">
-        <v>297</v>
       </c>
       <c r="E245" s="10" t="s">
         <v>459</v>
@@ -11572,10 +11580,10 @@
     </row>
     <row r="246" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C246" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E246" s="10" t="s">
         <v>459</v>
@@ -11583,10 +11591,10 @@
     </row>
     <row r="247" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C247" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E247" s="10" t="s">
         <v>459</v>
@@ -11594,49 +11602,59 @@
     </row>
     <row r="248" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="13" t="s">
+        <v>447</v>
+      </c>
+      <c r="C248" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="E248" s="10" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="13" t="s">
         <v>448</v>
       </c>
-      <c r="C248" s="13" t="s">
+      <c r="C249" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="E248" s="10" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="249" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="13" t="s">
+      <c r="E249" s="10" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="13" t="s">
         <v>449</v>
       </c>
-      <c r="C249" s="13" t="s">
+      <c r="C250" s="13" t="s">
         <v>450</v>
       </c>
-      <c r="E249" s="10" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="250" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="13" t="s">
+      <c r="E250" s="10" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="13" t="s">
         <v>451</v>
       </c>
-      <c r="C250" s="13" t="s">
+      <c r="C251" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="E250" s="10" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="251" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="13" t="s">
+      <c r="E251" s="10" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="13" t="s">
         <v>452</v>
       </c>
-      <c r="C251" s="13" t="s">
+      <c r="C252" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="E251" s="10" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E252" s="10" t="s">
+        <v>459</v>
+      </c>
+    </row>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
ccbottlersus fix survey Value2 display
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/Data/SurveyTemplateV2.xlsx
+++ b/Projects/CCBOTTLERSUS/Data/SurveyTemplateV2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -566,7 +566,7 @@
     <t xml:space="preserve">Value2</t>
   </si>
   <si>
-    <t xml:space="preserve">2: If there is a Sparkling display in this outlet, is display in best position?</t>
+    <t xml:space="preserve">2:Is there a Sparkling Display in this outlet?</t>
   </si>
   <si>
     <t xml:space="preserve">Value2a</t>
@@ -1648,7 +1648,7 @@
     <t xml:space="preserve">1a. Are Monster Energy products available in Coke FEM / FLM?</t>
   </si>
   <si>
-    <t xml:space="preserve">2:Is there a Sparkling Display in this outlet?</t>
+    <t xml:space="preserve">2: If there is a Sparkling display in this outlet, is display in best position?</t>
   </si>
   <si>
     <t xml:space="preserve">2: Is there a Sparkling Display in this outlet?</t>
@@ -2105,18 +2105,18 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A80" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K94" activeCellId="0" sqref="K94"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D87" activeCellId="0" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.2388663967611"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -4026,7 +4026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="s">
         <v>8</v>
       </c>
@@ -7665,15 +7665,15 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A84" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C89" activeCellId="0" sqref="C89"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A84" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C88" activeCellId="0" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="75.3036437246964"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="75.9473684210526"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -9064,10 +9064,10 @@
         <v>179</v>
       </c>
       <c r="B87" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C87" s="12" t="s">
         <v>540</v>
-      </c>
-      <c r="C87" s="12" t="s">
-        <v>180</v>
       </c>
       <c r="D87" s="18"/>
       <c r="E87" s="10" t="s">
@@ -9080,7 +9080,7 @@
         <v>179</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>540</v>
+        <v>180</v>
       </c>
       <c r="C88" s="12" t="s">
         <v>541</v>

</xml_diff>